<commit_message>
Working on revised network flow problem 4
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 02/Network Flow Graphs.xlsx
+++ b/03 - Homework/HW 02/Network Flow Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chickasawnation-my.sharepoint.com/personal/daniel_carpenter_chickasaw_net/Documents/Documents/GitHub/OU-DSA/Metaheuristics/03 - Homework/HW 02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="297" documentId="8_{DDE69595-AFB4-4123-BB98-2CC2CEAC48BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F3CC1761-E190-43A1-8B03-4BCE6554FB1A}"/>
+  <xr:revisionPtr revIDLastSave="650" documentId="8_{DDE69595-AFB4-4123-BB98-2CC2CEAC48BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{145DDE79-1534-4DC8-B7D9-8550D2538752}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t>Labor Sources</t>
   </si>
@@ -425,48 +425,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Utica,      Goggle   ]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Stamford,   Faceblock]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Stamford,   Goggle   ]</t>
-    </r>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -513,12 +471,33 @@
   <si>
     <t>Scranton, Utica, Stamford</t>
   </si>
+  <si>
+    <t>Prod</t>
+  </si>
+  <si>
+    <t>Scranton</t>
+  </si>
+  <si>
+    <t>Utica</t>
+  </si>
+  <si>
+    <t>Stamford</t>
+  </si>
+  <si>
+    <t>(0,0,0)</t>
+  </si>
+  <si>
+    <t>(1.5,0,100)</t>
+  </si>
+  <si>
+    <t>Maybe reverse this so that there is a 1.5 or 1 route before it gets to the arc with the cost.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,6 +557,26 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="3" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -608,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -659,6 +658,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,16 +688,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>339585</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>57978</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>420947</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114971</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>393919</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>137159</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>475281</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>194153</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -701,13 +709,13 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr>
-          <a:spLocks/>
+          <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5242889" y="1739348"/>
-          <a:ext cx="1280160" cy="1280159"/>
+          <a:off x="14943771" y="1560530"/>
+          <a:ext cx="1264569" cy="1255799"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -749,16 +757,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>331301</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>132521</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>357568</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>207108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>385635</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>211703</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>411901</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>50725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -770,13 +778,13 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr>
-          <a:spLocks/>
+          <a:spLocks noChangeAspect="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5234605" y="3495260"/>
-          <a:ext cx="1280160" cy="1280160"/>
+          <a:off x="13670156" y="4476549"/>
+          <a:ext cx="1264569" cy="1255558"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -819,14 +827,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>246822</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:colOff>197127</xdr:colOff>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>33131</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>362778</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:colOff>313083</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>132522</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -842,8 +850,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="859735" y="993914"/>
-          <a:ext cx="1341782" cy="1060173"/>
+          <a:off x="6293127" y="1014206"/>
+          <a:ext cx="1335156" cy="1051891"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartMagneticDisk">
           <a:avLst/>
@@ -913,14 +921,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>221974</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:colOff>197127</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>36444</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>337930</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:colOff>313083</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>135836</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -936,8 +944,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="834887" y="2678596"/>
-          <a:ext cx="1341782" cy="1060175"/>
+          <a:off x="6293127" y="2684394"/>
+          <a:ext cx="1335156" cy="1051892"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartMagneticDisk">
           <a:avLst/>
@@ -989,13 +997,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>197127</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>39757</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>313083</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>139148</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1011,8 +1019,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="810040" y="3882887"/>
-          <a:ext cx="1341782" cy="1060174"/>
+          <a:off x="6293127" y="4354582"/>
+          <a:ext cx="1335156" cy="1051891"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartMagneticDisk">
           <a:avLst/>
@@ -1064,13 +1072,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>314737</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>57977</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>369071</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>137158</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1133,13 +1141,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>306453</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>132520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>360787</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>211702</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1204,15 +1212,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>362778</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>82827</xdr:rowOff>
+      <xdr:colOff>313083</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>67639</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>339585</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>217667</xdr:rowOff>
+      <xdr:rowOff>82827</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1225,13 +1233,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="4" idx="4"/>
-          <a:endCxn id="2" idx="2"/>
+          <a:endCxn id="168" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2201517" y="1524001"/>
-          <a:ext cx="3041372" cy="855427"/>
+        <a:xfrm flipV="1">
+          <a:off x="7574495" y="1042551"/>
+          <a:ext cx="3917237" cy="1191805"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1260,15 +1268,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>337930</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>217667</xdr:rowOff>
+      <xdr:colOff>313083</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>130392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>339585</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>86141</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>86140</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1281,13 +1289,69 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="5" idx="4"/>
-          <a:endCxn id="2" idx="2"/>
+          <a:endCxn id="170" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2176669" y="2379428"/>
-          <a:ext cx="3066220" cy="829256"/>
+          <a:off x="7574495" y="2046598"/>
+          <a:ext cx="3917237" cy="1838336"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>313083</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>193145</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>89453</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85D481EA-55E4-406A-8340-8448367CB84A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="4"/>
+          <a:endCxn id="171" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7574495" y="3050645"/>
+          <a:ext cx="3917237" cy="2484867"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1318,69 +1382,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>313083</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>217667</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>339585</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>89453</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85D481EA-55E4-406A-8340-8448367CB84A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="6" idx="4"/>
-          <a:endCxn id="2" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2151822" y="2379428"/>
-          <a:ext cx="3091067" cy="2513938"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>362778</xdr:colOff>
-      <xdr:row>6</xdr:row>
       <xdr:rowOff>82827</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>331301</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>52014</xdr:rowOff>
+      <xdr:rowOff>20574</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1393,13 +1401,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="4" idx="4"/>
-          <a:endCxn id="3" idx="2"/>
+          <a:endCxn id="172" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2201517" y="1524001"/>
-          <a:ext cx="3033088" cy="2611339"/>
+          <a:off x="7574495" y="2234356"/>
+          <a:ext cx="3917237" cy="1820336"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1428,15 +1436,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>337930</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>86141</xdr:rowOff>
+      <xdr:colOff>313083</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>86140</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>331301</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>52014</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>83327</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1449,13 +1457,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="5" idx="4"/>
-          <a:endCxn id="3" idx="2"/>
+          <a:endCxn id="174" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2176669" y="3208684"/>
-          <a:ext cx="3057936" cy="926656"/>
+          <a:off x="7574495" y="3884934"/>
+          <a:ext cx="3917237" cy="1173805"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1485,14 +1493,14 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>313083</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>52014</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>89453</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>331301</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>89453</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>146079</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1505,13 +1513,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="6" idx="4"/>
-          <a:endCxn id="3" idx="2"/>
+          <a:endCxn id="175" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="2151822" y="4135340"/>
-          <a:ext cx="3082783" cy="758026"/>
+        <a:xfrm>
+          <a:off x="7574495" y="5535512"/>
+          <a:ext cx="3917237" cy="527273"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1541,14 +1549,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>369071</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>82827</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>246822</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>217666</xdr:rowOff>
+      <xdr:colOff>197127</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>216630</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1566,8 +1574,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3433636" y="1524001"/>
-          <a:ext cx="2942316" cy="855426"/>
+          <a:off x="3417071" y="1540152"/>
+          <a:ext cx="2876056" cy="848178"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1597,14 +1605,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>369071</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>217666</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>216630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>221974</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>86141</xdr:rowOff>
+      <xdr:colOff>197127</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>86140</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1622,8 +1630,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3433636" y="2379427"/>
-          <a:ext cx="2917468" cy="829257"/>
+          <a:off x="3417071" y="2388330"/>
+          <a:ext cx="2876056" cy="822010"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1653,13 +1661,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>369071</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>217666</xdr:rowOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>216630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>197127</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>89453</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1678,8 +1686,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3433636" y="2379427"/>
-          <a:ext cx="2892621" cy="2513939"/>
+          <a:off x="3417071" y="2388330"/>
+          <a:ext cx="2876056" cy="2492198"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1709,14 +1717,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>360787</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>82827</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>246822</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>52013</xdr:rowOff>
+      <xdr:colOff>197127</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>53049</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1734,8 +1742,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3425352" y="1524001"/>
-          <a:ext cx="2950600" cy="2611338"/>
+          <a:off x="3408787" y="1540152"/>
+          <a:ext cx="2884340" cy="2589597"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1765,14 +1773,14 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>360787</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>86141</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>86140</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>221974</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>52013</xdr:rowOff>
+      <xdr:colOff>197127</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>53049</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1790,8 +1798,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3425352" y="3208684"/>
-          <a:ext cx="2925752" cy="926655"/>
+          <a:off x="3408787" y="3210340"/>
+          <a:ext cx="2884340" cy="919409"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1821,13 +1829,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>360787</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>52013</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>53049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>197127</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>89453</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1846,8 +1854,1509 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3425352" y="4135339"/>
-          <a:ext cx="2900905" cy="758027"/>
+          <a:off x="3408787" y="4129749"/>
+          <a:ext cx="2884340" cy="750779"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>581685</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>56372</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>92524</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>393791</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Oval 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DD7BEC7-6424-4CC9-BDA7-62BB93A0EF90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11473803" y="6914372"/>
+          <a:ext cx="1326192" cy="1278713"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>dummy</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>313083</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>82827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>581685</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>225082</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="Straight Arrow Connector 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{263AA394-6315-4191-91E7-381ABE9739BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="4" idx="4"/>
+          <a:endCxn id="52" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7574495" y="2234356"/>
+          <a:ext cx="3899308" cy="5319373"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="lgDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>313083</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>86140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>581685</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>225082</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="70" name="Straight Arrow Connector 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{695D93D8-ED00-4B1F-8EB2-3EAEB62F6B3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="5" idx="4"/>
+          <a:endCxn id="52" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7574495" y="3884934"/>
+          <a:ext cx="3899308" cy="3668795"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="lgDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>313083</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>89453</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>581685</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>225082</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Straight Arrow Connector 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2A15FC7-48A4-44E3-8DA8-E6DFDB055E86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
+          <a:stCxn id="6" idx="4"/>
+          <a:endCxn id="52" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7574495" y="5535512"/>
+          <a:ext cx="3899308" cy="2018217"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="lgDash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>141536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>229065</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="168" name="Oval 167">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2FB5F21-E1D3-489F-AEA7-4BBA4B822CE6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11491732" y="645801"/>
+          <a:ext cx="822960" cy="793499"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>dumScGog</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>204289</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>56494</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="170" name="Oval 169">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{346A07BB-6B2F-4225-AC83-6EF50B77B6AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11491732" y="1649848"/>
+          <a:ext cx="822960" cy="793499"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>dumScGog</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>31719</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>119247</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="171" name="Oval 170">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F054D7E4-E6A0-4E31-8FAB-A2DBBE882C0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11491732" y="2653895"/>
+          <a:ext cx="822960" cy="793499"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>dumScGog</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>94471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>182000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="172" name="Oval 171">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0021BF88-CFC9-4FFB-AF0C-455D495C6E0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11491732" y="3657942"/>
+          <a:ext cx="822960" cy="793499"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>dumScFac</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>157224</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9429</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="174" name="Oval 173">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D75C645-70A3-4A43-B464-503BFCABB226}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11491732" y="4661989"/>
+          <a:ext cx="822960" cy="793499"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>dumScFac</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>599614</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>219976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>72181</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="175" name="Oval 174">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1EFC248B-F5AA-4057-9071-824703F2BD2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11491732" y="5666035"/>
+          <a:ext cx="822960" cy="793499"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>dumScFac</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>67639</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>1022</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>10245</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="185" name="Straight Arrow Connector 184">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B55DF57-108B-4722-A37C-F4F0D986F65C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="168" idx="6"/>
+          <a:endCxn id="2" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12314692" y="1042551"/>
+          <a:ext cx="2814271" cy="1589870"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>67639</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>1022</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>63556</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="189" name="Straight Arrow Connector 188">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2F59020-0547-4395-919D-66F145920B93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="168" idx="6"/>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12314692" y="1042551"/>
+          <a:ext cx="2814271" cy="701887"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>63556</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>1022</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>130392</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="192" name="Straight Arrow Connector 191">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0EBA085-24F3-456E-94C1-CCA89F577A8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="170" idx="6"/>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12314692" y="1744438"/>
+          <a:ext cx="2814271" cy="302160"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>130392</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>1022</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>10245</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="196" name="Straight Arrow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB801B1A-E3DA-4D54-AB7B-1C2244B4146E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="170" idx="6"/>
+          <a:endCxn id="2" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12314692" y="2046598"/>
+          <a:ext cx="2814271" cy="585823"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>63556</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>1022</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>193145</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="199" name="Straight Arrow Connector 198">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EBDDFA4-F2E2-494C-95AD-F4DC26A5109C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="171" idx="6"/>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12314692" y="1744438"/>
+          <a:ext cx="2814271" cy="1306207"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>10245</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>1022</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>193145</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="202" name="Straight Arrow Connector 201">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A0CE358-C20E-4954-AD94-339E26E3E994}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="171" idx="6"/>
+          <a:endCxn id="2" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12314692" y="2632421"/>
+          <a:ext cx="2814271" cy="418224"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>20574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>542760</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>155656</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="205" name="Straight Arrow Connector 204">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50169F97-5CE1-484F-B8D7-F25EE41A3791}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="172" idx="6"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12314692" y="4054692"/>
+          <a:ext cx="2750892" cy="605729"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>20574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>542760</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>102176</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="208" name="Straight Arrow Connector 207">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22C894A1-CE69-446A-9C01-17493352D1D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="172" idx="6"/>
+          <a:endCxn id="3" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12314692" y="4054692"/>
+          <a:ext cx="2750892" cy="1493543"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>155656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>542760</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>83327</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="211" name="Straight Arrow Connector 210">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2CD5D82-3DA9-44F7-A288-0A6CF7F506BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="174" idx="6"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12314692" y="4660421"/>
+          <a:ext cx="2750892" cy="398318"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>83327</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>542760</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>102176</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="214" name="Straight Arrow Connector 213">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A10B2508-1CD2-4DC8-8555-0DF92D2D4787}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="174" idx="6"/>
+          <a:endCxn id="3" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12314692" y="5058739"/>
+          <a:ext cx="2750892" cy="489496"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>155656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>542760</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>146079</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="217" name="Straight Arrow Connector 216">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2CC10AE-23A1-4D88-963F-A58A535B574E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="175" idx="6"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12314692" y="4660421"/>
+          <a:ext cx="2750892" cy="1402364"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>212339</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>102176</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>542760</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>146079</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="220" name="Straight Arrow Connector 219">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948448EE-968B-4E07-85A3-A37D903BED50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="175" idx="6"/>
+          <a:endCxn id="3" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="12314692" y="5548235"/>
+          <a:ext cx="2750892" cy="514550"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2173,10 +3682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63517073-B66B-40C8-B48B-0323E1700D94}">
-  <dimension ref="A1:AE42"/>
+  <dimension ref="A1:AI50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL14" sqref="AL14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -2194,13 +3703,13 @@
     <col min="32" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:29" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" s="12" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="C2" s="13"/>
       <c r="D2" s="14"/>
       <c r="E2" s="15" t="s">
@@ -2219,647 +3728,898 @@
       <c r="T2" s="15"/>
       <c r="AB2" s="17"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="C4" s="3"/>
-      <c r="L4" s="1">
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="C5" s="3"/>
+      <c r="R5" s="3" t="str">
+        <f>"(" &amp; 90 + 8 &amp;  "," &amp; "0,"  &amp; 0 &amp; ")"</f>
+        <v>(98,0,0)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="C6" s="3"/>
+      <c r="U6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG6" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="C7" s="3"/>
+      <c r="L7" s="1">
         <v>0</v>
       </c>
-      <c r="W4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y4" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="X7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AA4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>46</v>
+      <c r="AA7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C5" s="3"/>
-      <c r="V5" s="16" t="s">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="C8" s="3"/>
+      <c r="V8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="W5" s="1">
-        <f t="shared" ref="W5:W7" si="0">$F$27</f>
+      <c r="W8" s="1">
+        <f>$F$35</f>
         <v>166.7</v>
       </c>
-      <c r="X5" s="1">
+      <c r="X8" s="1">
         <v>300</v>
       </c>
-      <c r="Y5" s="1">
-        <f>W5 + X5</f>
+      <c r="Y8" s="1">
+        <f>W8 + X8</f>
         <v>466.7</v>
       </c>
-      <c r="Z5" s="1">
-        <f>VLOOKUP(W5, $F$27:$G$28, 2, FALSE)</f>
+      <c r="Z8" s="1">
+        <f>VLOOKUP(W8, $F$35:$G$36, 2, FALSE)</f>
         <v>100</v>
       </c>
-      <c r="AA5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB5" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(CHAR(9), FALSE, Y5:AA5)</f>
+      <c r="AA8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB8" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(CHAR(9), FALSE, Y8:AA8)</f>
         <v>466.7	100	.</v>
       </c>
-      <c r="AC5" s="1" t="str">
-        <f>V5 &amp; " " &amp; AB5</f>
+      <c r="AC8" s="1" t="str">
+        <f>V8 &amp; " " &amp; AB8</f>
         <v>[Specialist, Scranton ] 466.7	100	.</v>
       </c>
+      <c r="AE8" s="22" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C6" s="3"/>
-      <c r="V6" s="16" t="s">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="C9" s="3"/>
+      <c r="V9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="W6" s="1">
+      <c r="W9" s="1">
+        <f>$F$35</f>
+        <v>166.7</v>
+      </c>
+      <c r="X9" s="1">
+        <v>250</v>
+      </c>
+      <c r="Y9" s="1">
+        <f t="shared" ref="Y9:Y19" si="0">W9 + X9</f>
+        <v>416.7</v>
+      </c>
+      <c r="Z9" s="1">
+        <f>VLOOKUP(W9, $F$35:$G$36, 2, FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB9" s="2" t="str">
+        <f t="shared" ref="AB9:AB19" si="1">_xlfn.TEXTJOIN(CHAR(9), FALSE, Y9:AA9)</f>
+        <v>416.7	100	.</v>
+      </c>
+      <c r="AC9" s="1" t="str">
+        <f t="shared" ref="AC9:AC19" si="2">V9 &amp; " " &amp; AB9</f>
+        <v>[Specialist, Utica    ] 416.7	100	.</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="C10" s="3"/>
+      <c r="E10" s="1">
+        <f>E35 * G35</f>
+        <v>1200</v>
+      </c>
+      <c r="R10" s="3" t="str">
+        <f>"(" &amp; 105+14 &amp;  "," &amp; "0,"  &amp; 0 &amp; ")"</f>
+        <v>(119,0,0)</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="V10" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="W10" s="1">
+        <f>$F$35</f>
+        <v>166.7</v>
+      </c>
+      <c r="X10" s="1">
+        <v>275</v>
+      </c>
+      <c r="Y10" s="1">
         <f t="shared" si="0"/>
-        <v>166.7</v>
-      </c>
-      <c r="X6" s="1">
+        <v>441.7</v>
+      </c>
+      <c r="Z10" s="1">
+        <f>VLOOKUP(W10, $F$35:$G$36, 2, FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>441.7	100	.</v>
+      </c>
+      <c r="AC10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>[Specialist, Stamford ] 441.7	100	.</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="C11" s="3"/>
+      <c r="H11" s="3" t="str">
+        <f>"(" &amp; 300 + $F$35 &amp;  "," &amp; "0,"  &amp; $G$35 &amp; ")"</f>
+        <v>(466.7,0,100)</v>
+      </c>
+      <c r="V11" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="W11" s="1">
+        <f>$F$36</f>
+        <v>170</v>
+      </c>
+      <c r="X11" s="1">
+        <f>X8</f>
+        <v>300</v>
+      </c>
+      <c r="Y11" s="1">
+        <f t="shared" si="0"/>
+        <v>470</v>
+      </c>
+      <c r="Z11" s="1">
+        <f>VLOOKUP(W11, $F$35:$G$36, 2, FALSE)</f>
+        <v>200</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>470	200	.</v>
+      </c>
+      <c r="AC11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>[Generalist, Scranton ] 470	200	.</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="C12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="U12" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="V12" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="W12" s="1">
+        <f>$F$36</f>
+        <v>170</v>
+      </c>
+      <c r="X12" s="1">
+        <f t="shared" ref="X12:X13" si="3">X9</f>
         <v>250</v>
       </c>
-      <c r="Y6" s="1">
-        <f t="shared" ref="Y6:Y16" si="1">W6 + X6</f>
-        <v>416.7</v>
-      </c>
-      <c r="Z6" s="1">
-        <f t="shared" ref="Z6:Z10" si="2">VLOOKUP(W6, $F$27:$G$28, 2, FALSE)</f>
-        <v>100</v>
-      </c>
-      <c r="AA6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB6" s="2" t="str">
-        <f t="shared" ref="AB6:AB16" si="3">_xlfn.TEXTJOIN(CHAR(9), FALSE, Y6:AA6)</f>
-        <v>416.7	100	.</v>
-      </c>
-      <c r="AC6" s="1" t="str">
-        <f t="shared" ref="AC6:AC16" si="4">V6 &amp; " " &amp; AB6</f>
-        <v>[Specialist, Utica    ] 416.7	100	.</v>
+      <c r="Y12" s="1">
+        <f t="shared" si="0"/>
+        <v>420</v>
+      </c>
+      <c r="Z12" s="1">
+        <f>VLOOKUP(W12, $F$35:$G$36, 2, FALSE)</f>
+        <v>200</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>420	200	.</v>
+      </c>
+      <c r="AC12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>[Generalist, Utica    ] 420	200	.</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C7" s="3"/>
-      <c r="O7" s="3" t="str">
-        <f>"(" &amp; 90 + 8 &amp;  "," &amp; "0,"  &amp; 505 &amp; ")"</f>
-        <v>(98,0,505)</v>
-      </c>
-      <c r="S7" s="1">
-        <v>-1000</v>
-      </c>
-      <c r="V7" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="W7" s="1">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="C13" s="3"/>
+      <c r="J13" s="2" t="str">
+        <f>"(" &amp; 300 + $F$36 &amp;  "," &amp; "0,"  &amp; $G$36 &amp; ")"</f>
+        <v>(470,0,200)</v>
+      </c>
+      <c r="V13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W13" s="1">
+        <f>$F$36</f>
+        <v>170</v>
+      </c>
+      <c r="X13" s="1">
+        <f t="shared" si="3"/>
+        <v>275</v>
+      </c>
+      <c r="Y13" s="1">
         <f t="shared" si="0"/>
-        <v>166.7</v>
-      </c>
-      <c r="X7" s="1">
-        <v>275</v>
-      </c>
-      <c r="Y7" s="1">
+        <v>445</v>
+      </c>
+      <c r="Z13" s="1">
+        <f>VLOOKUP(W13, $F$35:$G$36, 2, FALSE)</f>
+        <v>200</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>441.7</v>
-      </c>
-      <c r="Z7" s="1">
+        <v>445	200	.</v>
+      </c>
+      <c r="AC13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="AA7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB7" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>441.7	100	.</v>
-      </c>
-      <c r="AC7" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>[Specialist, Stamford ] 441.7	100	.</v>
+        <v>[Generalist, Stamford ] 445	200	.</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C8" s="3"/>
-      <c r="H8" s="3" t="str">
-        <f>"(" &amp; 300 + $F$27 &amp;  "," &amp; "0,"  &amp; $G$27 &amp; ")"</f>
-        <v>(466.7,0,100)</v>
-      </c>
-      <c r="V8" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="W8" s="1">
-        <f t="shared" ref="W8:W10" si="5">$F$28</f>
-        <v>170</v>
-      </c>
-      <c r="X8" s="1">
-        <f>X5</f>
-        <v>300</v>
-      </c>
-      <c r="Y8" s="1">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="C14" s="3"/>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="R14" s="4" t="str">
+        <f>"(" &amp; 115+24 &amp;  "," &amp; "0,"  &amp; 0 &amp; ")"</f>
+        <v>(139,0,0)</v>
+      </c>
+      <c r="V14" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="W14" s="1">
+        <v>90</v>
+      </c>
+      <c r="X14" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y14" s="1">
+        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>505</v>
+      </c>
+      <c r="AA14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>470</v>
-      </c>
-      <c r="Z8" s="1">
+        <v>98	505	.</v>
+      </c>
+      <c r="AC14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="AA8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB8" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>470	200	.</v>
-      </c>
-      <c r="AC8" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>[Generalist, Scranton ] 470	200	.</v>
+        <v>[Scranton,   Faceblock] 98	505	.</v>
+      </c>
+      <c r="AE14" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="V9" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="W9" s="1">
-        <f t="shared" si="5"/>
-        <v>170</v>
-      </c>
-      <c r="X9" s="1">
-        <f t="shared" ref="X9:X10" si="6">X6</f>
-        <v>250</v>
-      </c>
-      <c r="Y9" s="1">
-        <f t="shared" si="1"/>
-        <v>420</v>
-      </c>
-      <c r="Z9" s="1">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="AA9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB9" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>420	200	.</v>
-      </c>
-      <c r="AC9" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>[Generalist, Utica    ] 420	200	.</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C10" s="3"/>
-      <c r="J10" s="2" t="str">
-        <f>"(" &amp; 300 + $F$28 &amp;  "," &amp; "0,"  &amp; $G$28 &amp; ")"</f>
-        <v>(470,0,200)</v>
-      </c>
-      <c r="N10" s="3" t="str">
-        <f>"(" &amp; 90+15  &amp;  "," &amp; "0,"  &amp; 505 &amp; ")"</f>
-        <v>(105,0,505)</v>
-      </c>
-      <c r="V10" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="W10" s="1">
-        <f t="shared" si="5"/>
-        <v>170</v>
-      </c>
-      <c r="X10" s="1">
-        <f t="shared" si="6"/>
-        <v>275</v>
-      </c>
-      <c r="Y10" s="1">
-        <f t="shared" si="1"/>
-        <v>445</v>
-      </c>
-      <c r="Z10" s="1">
-        <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="AA10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB10" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>445	200	.</v>
-      </c>
-      <c r="AC10" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>[Generalist, Stamford ] 445	200	.</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C11" s="3"/>
-      <c r="L11" s="1">
-        <v>0</v>
-      </c>
-      <c r="V11" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="W11" s="1">
-        <v>90</v>
-      </c>
-      <c r="X11" s="1">
-        <v>8</v>
-      </c>
-      <c r="Y11" s="1">
-        <f t="shared" si="1"/>
-        <v>98</v>
-      </c>
-      <c r="Z11" s="1">
-        <v>505</v>
-      </c>
-      <c r="AA11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB11" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>98	505	.</v>
-      </c>
-      <c r="AC11" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>[Scranton,   Faceblock] 98	505	.</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C12" s="3"/>
-      <c r="J12" s="3" t="str">
-        <f>"(" &amp; 250 + $F$27 &amp;  "," &amp; "0,"  &amp; $G$27 &amp; ")"</f>
-        <v>(416.7,0,100)</v>
-      </c>
-      <c r="N12" s="1" t="str">
-        <f>"(" &amp; 105+14 &amp;  "," &amp; "0,"  &amp; 465 &amp; ")"</f>
-        <v>(119,0,465)</v>
-      </c>
-      <c r="V12" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="W12" s="1">
-        <f>W11</f>
-        <v>90</v>
-      </c>
-      <c r="X12" s="1">
-        <v>15</v>
-      </c>
-      <c r="Y12" s="1">
-        <f t="shared" si="1"/>
-        <v>105</v>
-      </c>
-      <c r="Z12" s="1">
-        <f>Z11</f>
-        <v>505</v>
-      </c>
-      <c r="AA12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB12" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>105	505	.</v>
-      </c>
-      <c r="AC12" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>[Scranton,   Goggle   ] 105	505	.</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C13" s="3"/>
-      <c r="V13" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="W13" s="1">
-        <v>105</v>
-      </c>
-      <c r="X13" s="1">
-        <v>14</v>
-      </c>
-      <c r="Y13" s="1">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="Z13" s="1">
-        <v>465</v>
-      </c>
-      <c r="AA13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB13" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>119	465	.</v>
-      </c>
-      <c r="AC13" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>[Utica,      Faceblock] 119	465	.</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="C14" s="3"/>
-      <c r="V14" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="W14" s="1">
-        <f>W13</f>
-        <v>105</v>
-      </c>
-      <c r="X14" s="1">
-        <v>18</v>
-      </c>
-      <c r="Y14" s="1">
-        <f t="shared" si="1"/>
-        <v>123</v>
-      </c>
-      <c r="Z14" s="1">
-        <f>Z13</f>
-        <v>465</v>
-      </c>
-      <c r="AA14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB14" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>123	465	.</v>
-      </c>
-      <c r="AC14" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>[Utica,      Goggle   ] 123	465	.</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="C15" s="3"/>
       <c r="J15" s="3" t="str">
-        <f>"(" &amp; 250 + $F$28 &amp;  "," &amp; "0,"  &amp; $G$28 &amp; ")"</f>
-        <v>(420,0,200)</v>
-      </c>
-      <c r="N15" s="3" t="str">
-        <f>"(" &amp; 105+18 &amp;  "," &amp; "0,"  &amp; 465 &amp; ")"</f>
-        <v>(123,0,465)</v>
+        <f>"(" &amp; 250 + $F$35 &amp;  "," &amp; "0,"  &amp; $G$35 &amp; ")"</f>
+        <v>(416.7,0,100)</v>
       </c>
       <c r="V15" s="16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="W15" s="1">
-        <v>115</v>
+        <f>W14</f>
+        <v>90</v>
       </c>
       <c r="X15" s="1">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="Y15" s="1">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="Z15" s="1">
+        <f>Z14</f>
+        <v>505</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>139</v>
-      </c>
-      <c r="Z15" s="1">
-        <v>570</v>
-      </c>
-      <c r="AA15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB15" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>139	570	.</v>
+        <v>105	505	.</v>
       </c>
       <c r="AC15" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>[Stamford,   Faceblock] 139	570	.</v>
+        <f t="shared" si="2"/>
+        <v>[Scranton,   Goggle   ] 105	505	.</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="C16" s="3"/>
       <c r="V16" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="W16" s="1">
+        <v>105</v>
+      </c>
+      <c r="X16" s="1">
+        <v>14</v>
+      </c>
+      <c r="Y16" s="1">
+        <f t="shared" si="0"/>
+        <v>119</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>465</v>
+      </c>
+      <c r="AA16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="W16" s="1">
-        <f>W15</f>
-        <v>115</v>
-      </c>
-      <c r="X16" s="1">
-        <v>20</v>
-      </c>
-      <c r="Y16" s="1">
+      <c r="AB16" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>135</v>
-      </c>
-      <c r="Z16" s="1">
-        <f>Z15</f>
-        <v>570</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB16" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>135	570	.</v>
+        <v>119	465	.</v>
       </c>
       <c r="AC16" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>[Stamford,   Goggle   ] 135	570	.</v>
+        <f t="shared" si="2"/>
+        <v>[Utica,      Faceblock] 119	465	.</v>
       </c>
     </row>
-    <row r="17" spans="3:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="3:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:35" x14ac:dyDescent="0.3">
       <c r="C18" s="3"/>
-      <c r="J18" s="2" t="str">
-        <f>"(" &amp; 275 + $F$27 &amp;  "," &amp; "0,"  &amp; $G$27 &amp; ")"</f>
+      <c r="J18" s="3" t="str">
+        <f>"(" &amp; 250 + $F$36 &amp;  "," &amp; "0,"  &amp; $G$36 &amp; ")"</f>
+        <v>(420,0,200)</v>
+      </c>
+      <c r="S18" s="3" t="str">
+        <f>"(" &amp; 90+15  &amp;  "," &amp; "0,"  &amp; 0 &amp; ")"</f>
+        <v>(105,0,0)</v>
+      </c>
+    </row>
+    <row r="19" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="C19" s="3"/>
+      <c r="U19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG19" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="C20" s="3"/>
+      <c r="R20" s="3" t="str">
+        <f>"(" &amp; 105+18 &amp;  "," &amp; "0,"  &amp; 0 &amp; ")"</f>
+        <v>(123,0,0)</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="C21" s="3"/>
+      <c r="J21" s="2" t="str">
+        <f>"(" &amp; 275 + $F$35 &amp;  "," &amp; "0,"  &amp; $G$35 &amp; ")"</f>
         <v>(441.7,0,100)</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L21" s="1">
         <v>0</v>
       </c>
-      <c r="N18" s="3" t="str">
-        <f>"(" &amp; 115+24 &amp;  "," &amp; "0,"  &amp; 570 &amp; ")"</f>
-        <v>(139,0,570)</v>
+      <c r="V21" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="W21" s="1">
+        <f>$F$35</f>
+        <v>166.7</v>
+      </c>
+      <c r="X21" s="1">
+        <v>300</v>
+      </c>
+      <c r="Y21" s="1">
+        <f>W21 + X21</f>
+        <v>466.7</v>
+      </c>
+      <c r="Z21" s="1">
+        <f>VLOOKUP(W21, $F$35:$G$36, 2, FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB21" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(CHAR(9), FALSE, Y21:AA21)</f>
+        <v>466.7	100	.</v>
+      </c>
+      <c r="AC21" s="1" t="str">
+        <f>V21 &amp; " " &amp; AB21</f>
+        <v>[Specialist, Scranton ] 466.7	100	.</v>
+      </c>
+      <c r="AE21" s="22" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="19" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C19" s="3"/>
+    <row r="22" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="C22" s="3"/>
+      <c r="V22" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="W22" s="1">
+        <f>$F$35</f>
+        <v>166.7</v>
+      </c>
+      <c r="X22" s="1">
+        <v>250</v>
+      </c>
+      <c r="Y22" s="1">
+        <f t="shared" ref="Y22:Y27" si="4">W22 + X22</f>
+        <v>416.7</v>
+      </c>
+      <c r="Z22" s="1">
+        <f>VLOOKUP(W22, $F$35:$G$36, 2, FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB22" s="2" t="str">
+        <f t="shared" ref="AB22:AB27" si="5">_xlfn.TEXTJOIN(CHAR(9), FALSE, Y22:AA22)</f>
+        <v>416.7	100	.</v>
+      </c>
+      <c r="AC22" s="1" t="str">
+        <f t="shared" ref="AC22:AC27" si="6">V22 &amp; " " &amp; AB22</f>
+        <v>[Specialist, Utica    ] 416.7	100	.</v>
+      </c>
     </row>
-    <row r="20" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C20" s="3"/>
-      <c r="H20" s="2" t="str">
-        <f>"(" &amp; 275 + $F$28 &amp;  "," &amp; "0,"  &amp; $G$28 &amp; ")"</f>
+    <row r="23" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="C23" s="3"/>
+      <c r="H23" s="2" t="str">
+        <f>"(" &amp; 275 + $F$36 &amp;  "," &amp; "0,"  &amp; $G$36 &amp; ")"</f>
         <v>(445,0,200)</v>
       </c>
+      <c r="U23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="V23" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="W23" s="1">
+        <f>$F$35</f>
+        <v>166.7</v>
+      </c>
+      <c r="X23" s="1">
+        <v>275</v>
+      </c>
+      <c r="Y23" s="1">
+        <f t="shared" si="4"/>
+        <v>441.7</v>
+      </c>
+      <c r="Z23" s="1">
+        <f>VLOOKUP(W23, $F$35:$G$36, 2, FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="AA23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB23" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>441.7	100	.</v>
+      </c>
+      <c r="AC23" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>[Specialist, Stamford ] 441.7	100	.</v>
+      </c>
     </row>
-    <row r="21" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C21" s="3"/>
-      <c r="N21" s="2" t="str">
-        <f>"(" &amp; 115+20 &amp;  "," &amp; "0,"  &amp; 570 &amp; ")"</f>
-        <v>(135,0,570)</v>
-      </c>
-      <c r="S21" s="1">
+    <row r="24" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="C24" s="3"/>
+      <c r="E24" s="1">
+        <f>E36 * G36</f>
+        <v>2000</v>
+      </c>
+      <c r="V24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="W24" s="1">
+        <f>$F$36</f>
+        <v>170</v>
+      </c>
+      <c r="X24" s="1">
+        <f>X21</f>
+        <v>300</v>
+      </c>
+      <c r="Y24" s="1">
+        <f t="shared" si="4"/>
+        <v>470</v>
+      </c>
+      <c r="Z24" s="1">
+        <f>VLOOKUP(W24, $F$35:$G$36, 2, FALSE)</f>
+        <v>200</v>
+      </c>
+      <c r="AA24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB24" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>470	200	.</v>
+      </c>
+      <c r="AC24" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>[Generalist, Scranton ] 470	200	.</v>
+      </c>
+    </row>
+    <row r="25" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="C25" s="3"/>
+      <c r="I25" s="20"/>
+      <c r="R25" s="2" t="str">
+        <f>"(" &amp; 115+20 &amp;  "," &amp; "0,"  &amp; 0 &amp; ")"</f>
+        <v>(135,0,0)</v>
+      </c>
+      <c r="U25" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="V25" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="W25" s="1">
+        <f>$F$36</f>
+        <v>170</v>
+      </c>
+      <c r="X25" s="1">
+        <f t="shared" ref="X25:X26" si="7">X22</f>
+        <v>250</v>
+      </c>
+      <c r="Y25" s="1">
+        <f t="shared" si="4"/>
+        <v>420</v>
+      </c>
+      <c r="Z25" s="1">
+        <f>VLOOKUP(W25, $F$35:$G$36, 2, FALSE)</f>
+        <v>200</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB25" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>420	200	.</v>
+      </c>
+      <c r="AC25" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>[Generalist, Utica    ] 420	200	.</v>
+      </c>
+      <c r="AI25" s="1">
         <v>-600</v>
       </c>
     </row>
-    <row r="22" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C22" s="3"/>
+    <row r="26" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="C26" s="3"/>
+      <c r="V26" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W26" s="1">
+        <f>$F$36</f>
+        <v>170</v>
+      </c>
+      <c r="X26" s="1">
+        <f t="shared" si="7"/>
+        <v>275</v>
+      </c>
+      <c r="Y26" s="1">
+        <f t="shared" si="4"/>
+        <v>445</v>
+      </c>
+      <c r="Z26" s="1">
+        <f>VLOOKUP(W26, $F$35:$G$36, 2, FALSE)</f>
+        <v>200</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB26" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>445	200	.</v>
+      </c>
+      <c r="AC26" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>[Generalist, Stamford ] 445	200	.</v>
+      </c>
     </row>
-    <row r="23" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C23" s="3"/>
+    <row r="27" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="C27" s="3"/>
+      <c r="Q27" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="V27" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="W27" s="1">
+        <v>90</v>
+      </c>
+      <c r="X27" s="1">
+        <v>8</v>
+      </c>
+      <c r="Y27" s="1">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="Z27" s="1">
+        <v>505</v>
+      </c>
+      <c r="AA27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB27" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>98	505	.</v>
+      </c>
+      <c r="AC27" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>[Scranton,   Faceblock] 98	505	.</v>
+      </c>
+      <c r="AE27" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="24" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C24" s="3"/>
+    <row r="28" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="C28" s="3"/>
+      <c r="S28" s="21" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="25" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C25" s="3"/>
+    <row r="29" spans="3:35" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="AB29" s="18"/>
     </row>
-    <row r="26" spans="3:28" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="C26" s="7"/>
-      <c r="D26" s="6" t="s">
+    <row r="30" spans="3:35" x14ac:dyDescent="0.3">
+      <c r="Q30" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI30" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="L33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E34" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G34" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AB26" s="18"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="27" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C27" s="3" t="s">
+    <row r="35" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C35" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D35" s="4">
         <v>2000</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E35" s="1">
         <v>12</v>
       </c>
-      <c r="F27" s="1">
-        <f>ROUND(D27 / E27, 1)</f>
+      <c r="F35" s="1">
+        <f>ROUND(D35 / E35, 1)</f>
         <v>166.7</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G35" s="1">
         <v>100</v>
       </c>
+      <c r="I35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" s="1">
+        <v>505</v>
+      </c>
+      <c r="U35" s="1">
+        <f>-(SUM(E24, E10) + SUM(AI25, AI6))</f>
+        <v>-1600</v>
+      </c>
     </row>
-    <row r="28" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C28" s="3" t="s">
+    <row r="36" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C36" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D36" s="4">
         <v>1700</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E36" s="1">
         <v>10</v>
       </c>
-      <c r="F28" s="1">
-        <f>ROUND(D28 / E28, 1)</f>
+      <c r="F36" s="1">
+        <f>ROUND(D36 / E36, 1)</f>
         <v>170</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G36" s="1">
         <v>200</v>
       </c>
+      <c r="I36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J36" s="1">
+        <v>465</v>
+      </c>
     </row>
-    <row r="29" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C29" s="3"/>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C37" s="3"/>
+      <c r="I37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J37" s="1">
+        <v>570</v>
+      </c>
     </row>
-    <row r="30" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C30" s="8" t="s">
+    <row r="38" spans="2:28" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="1"/>
+      <c r="C38" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="AB38" s="19"/>
     </row>
-    <row r="31" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C31" s="8" t="s">
+    <row r="39" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C39" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C32" s="8" t="s">
+    <row r="40" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C40" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="3:28" x14ac:dyDescent="0.3">
-      <c r="C33" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>51</v>
+    <row r="41" spans="2:28" x14ac:dyDescent="0.3">
+      <c r="C41" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="35" spans="3:28" s="11" customFormat="1" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="C35" s="9" t="s">
+    <row r="43" spans="2:28" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="B43" s="11"/>
+      <c r="C43" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D43" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AB35" s="19"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
     </row>
-    <row r="37" spans="3:28" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="C37" s="8" t="s">
+    <row r="45" spans="2:28" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="C45" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="3:28" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="C38" s="8" t="s">
+    <row r="46" spans="2:28" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="C46" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="3:28" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="C39" s="8" t="s">
+    <row r="47" spans="2:28" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="C47" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="3:28" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="C40" s="8" t="s">
+    <row r="48" spans="2:28" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="C48" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="3:28" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="C41" s="8" t="s">
+    <row r="49" spans="3:4" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="C49" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>49</v>
+      <c r="D49" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="42" spans="3:28" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="C42" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>48</v>
+    <row r="50" spans="3:4" ht="20.25" x14ac:dyDescent="0.35">
+      <c r="C50" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Format and change dummy cost = 0
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 02/Network Flow Graphs.xlsx
+++ b/03 - Homework/HW 02/Network Flow Graphs.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chickasawnation-my.sharepoint.com/personal/daniel_carpenter_chickasaw_net/Documents/Documents/GitHub/OU-DSA/Metaheuristics/03 - Homework/HW 02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1796" documentId="8_{DDE69595-AFB4-4123-BB98-2CC2CEAC48BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F50076C5-F834-4685-BAD3-E8D975C439CA}"/>
+  <xr:revisionPtr revIDLastSave="1905" documentId="8_{DDE69595-AFB4-4123-BB98-2CC2CEAC48BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{866ECA8E-3C33-4208-AB6D-26D79D47AC9F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE14DA27-A8C1-45F9-9C11-8787018CF8AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE14DA27-A8C1-45F9-9C11-8787018CF8AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem 4" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="158">
   <si>
     <t>Labor Sources</t>
   </si>
@@ -705,9 +705,6 @@
     <t>(123,0,∞)</t>
   </si>
   <si>
-    <t>Overtime Multiplier</t>
-  </si>
-  <si>
     <t>Nodes: Supply (Demand)</t>
   </si>
   <si>
@@ -864,9 +861,6 @@
     <t>[Stamford,   dummy   ]</t>
   </si>
   <si>
-    <t>(1000,0,∞)</t>
-  </si>
-  <si>
     <t>Concat</t>
   </si>
   <si>
@@ -900,9 +894,6 @@
     <t>;</t>
   </si>
   <si>
-    <t># 1200 + 2000 - 1000 - 600</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -925,6 +916,18 @@
   </si>
   <si>
     <t># Transshippment (Plants or OT Multiplier)</t>
+  </si>
+  <si>
+    <t>* *Mult includes *Mult1x and *MultOT for simiplicity in graph</t>
+  </si>
+  <si>
+    <t>Overtime Choice</t>
+  </si>
+  <si>
+    <t>(0,0,∞)</t>
+  </si>
+  <si>
+    <t># 1200 + 2000 - 0 - 600</t>
   </si>
 </sst>
 </file>
@@ -935,9 +938,9 @@
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1109,8 +1112,15 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1131,25 +1141,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1167,24 +1159,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
+        <fgColor theme="6" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1308,51 +1306,6 @@
         <color theme="0" tint="-0.14993743705557422"/>
       </right>
       <top style="thin">
-        <color theme="4" tint="0.39991454817346722"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14990691854609822"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14993743705557422"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14993743705557422"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39991454817346722"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14990691854609822"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14993743705557422"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14990691854609822"/>
-      </right>
-      <top style="thin">
-        <color theme="4" tint="0.39991454817346722"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14990691854609822"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14990691854609822"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14993743705557422"/>
-      </right>
-      <top style="thin">
         <color theme="0" tint="-0.14993743705557422"/>
       </top>
       <bottom style="thin">
@@ -1434,15 +1387,6 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="9" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
         <color theme="5" tint="-0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -1452,7 +1396,64 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="7" tint="-0.24994659260841701"/>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="3" tint="0.59996337778862885"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1461,7 +1462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1543,12 +1544,6 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1564,15 +1559,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1582,108 +1615,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1702,7 +1670,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1716,6 +1684,40 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1843,15 +1845,15 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
+          <a:schemeClr val="accent3">
             <a:shade val="50000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent3"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:schemeClr val="accent3"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -1879,14 +1881,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>197127</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>220909</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>30406</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>313083</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>75372</xdr:rowOff>
+      <xdr:rowOff>129684</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1901,8 +1903,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9381948" y="1255052"/>
-          <a:ext cx="1340599" cy="1079106"/>
+          <a:off x="7721877" y="1540799"/>
+          <a:ext cx="1340599" cy="1078992"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartMagneticDisk">
           <a:avLst/>
@@ -1943,27 +1945,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Scranton,</a:t>
+            <a:t>Scranton</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> PA</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2037,7 +2020,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Utica, NY</a:t>
+            <a:t>Utica</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2112,7 +2095,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Stamford, CT</a:t>
+            <a:t>Stamford</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2156,15 +2139,15 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent4">
+          <a:schemeClr val="accent1">
             <a:shade val="50000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent4"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -2225,15 +2208,15 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent6">
+          <a:schemeClr val="accent1">
             <a:shade val="50000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -2265,7 +2248,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>313083</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>25676</xdr:rowOff>
+      <xdr:rowOff>80045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
@@ -2290,8 +2273,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10722547" y="1794605"/>
-          <a:ext cx="3079825" cy="929142"/>
+          <a:off x="9062476" y="2080295"/>
+          <a:ext cx="4304468" cy="874774"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2436,7 +2419,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>313083</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>25676</xdr:rowOff>
+      <xdr:rowOff>80045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
@@ -2460,8 +2443,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10722547" y="1794605"/>
-          <a:ext cx="3079825" cy="2718186"/>
+          <a:off x="9062476" y="2080295"/>
+          <a:ext cx="4304468" cy="2663817"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2604,7 +2587,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>369071</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>25676</xdr:rowOff>
+      <xdr:rowOff>80045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -2628,8 +2611,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3430678" y="1794605"/>
-          <a:ext cx="2903270" cy="929141"/>
+          <a:off x="1770607" y="2080295"/>
+          <a:ext cx="2903270" cy="874773"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2772,7 +2755,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>360787</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>25676</xdr:rowOff>
+      <xdr:rowOff>80045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
@@ -2796,8 +2779,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3422394" y="1794605"/>
-          <a:ext cx="2911554" cy="2718185"/>
+          <a:off x="1762323" y="2080295"/>
+          <a:ext cx="2911554" cy="2663816"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3031,13 +3014,13 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>313083</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>25676</xdr:rowOff>
+      <xdr:rowOff>80045</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>331301</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>44963</xdr:rowOff>
+      <xdr:rowOff>44962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3056,8 +3039,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10722547" y="1794605"/>
-          <a:ext cx="3079825" cy="4672929"/>
+          <a:off x="9062476" y="2080295"/>
+          <a:ext cx="4304468" cy="4618560"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3222,14 +3205,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>210734</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>220909</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>30406</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>326690</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>75372</xdr:rowOff>
+      <xdr:rowOff>129684</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3244,8 +3227,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6333948" y="1255052"/>
-          <a:ext cx="1340599" cy="1079106"/>
+          <a:off x="4673877" y="1540799"/>
+          <a:ext cx="1340599" cy="1078992"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartMagneticDisk">
           <a:avLst/>
@@ -6804,11 +6787,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC69D54E-00BB-4469-9873-ACE66827EA4B}">
-  <dimension ref="A1:BN52"/>
+  <dimension ref="A1:BJ52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AQ29" sqref="AQ6:AQ29"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -6850,7 +6831,7 @@
       <c r="D2" s="15"/>
       <c r="I2" s="15"/>
       <c r="J2" s="15" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="K2" s="15"/>
       <c r="N2" s="15"/>
@@ -6865,14 +6846,14 @@
       <c r="Y2" s="15"/>
       <c r="Z2" s="26"/>
       <c r="AA2" s="1"/>
-      <c r="AB2" s="84" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84"/>
-      <c r="AF2" s="84"/>
-      <c r="AG2" s="84"/>
+      <c r="AB2" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC2" s="71"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
+      <c r="AF2" s="71"/>
+      <c r="AG2" s="71"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="2"/>
@@ -6880,11 +6861,11 @@
       <c r="AL2" s="26"/>
       <c r="AM2" s="26"/>
       <c r="AN2" s="26"/>
-      <c r="AO2" s="94"/>
+      <c r="AO2" s="81"/>
       <c r="AP2" s="26"/>
       <c r="AQ2" s="26"/>
-      <c r="AR2" s="88"/>
-      <c r="AS2" s="88"/>
+      <c r="AR2" s="75"/>
+      <c r="AS2" s="75"/>
       <c r="AT2" s="26"/>
       <c r="AU2" s="26"/>
       <c r="AV2" s="26"/>
@@ -6912,11 +6893,11 @@
       <c r="AL3" s="26"/>
       <c r="AM3" s="26"/>
       <c r="AN3" s="26"/>
-      <c r="AO3" s="94"/>
+      <c r="AO3" s="81"/>
       <c r="AP3" s="26"/>
       <c r="AQ3" s="26"/>
-      <c r="AR3" s="88"/>
-      <c r="AS3" s="88"/>
+      <c r="AR3" s="75"/>
+      <c r="AS3" s="75"/>
       <c r="AT3" s="26"/>
       <c r="AU3" s="26"/>
       <c r="AV3" s="26"/>
@@ -6928,14 +6909,14 @@
     <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="AA4" s="6"/>
-      <c r="AB4" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="AC4" s="31"/>
-      <c r="AD4" s="31"/>
-      <c r="AE4" s="31"/>
-      <c r="AF4" s="31"/>
-      <c r="AG4" s="31"/>
+      <c r="AB4" s="85" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC4" s="85"/>
+      <c r="AD4" s="85"/>
+      <c r="AE4" s="85"/>
+      <c r="AF4" s="85"/>
+      <c r="AG4" s="85"/>
     </row>
     <row r="5" spans="1:60" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -6945,23 +6926,23 @@
       <c r="O5" s="1">
         <v>0</v>
       </c>
-      <c r="AB5" s="33" t="s">
+      <c r="AB5" s="93" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC5" s="93" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD5" s="93" t="s">
         <v>97</v>
       </c>
-      <c r="AC5" s="33" t="s">
+      <c r="AE5" s="93" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF5" s="93" t="s">
         <v>99</v>
       </c>
-      <c r="AD5" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE5" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="AF5" s="33" t="s">
+      <c r="AG5" s="93" t="s">
         <v>100</v>
-      </c>
-      <c r="AG5" s="50" t="s">
-        <v>101</v>
       </c>
       <c r="AK5" s="32"/>
       <c r="AL5" s="32" t="s">
@@ -6974,10 +6955,10 @@
         <v>10</v>
       </c>
       <c r="AO5" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="AQ5" s="90" t="s">
-        <v>137</v>
+        <v>146</v>
+      </c>
+      <c r="AQ5" s="77" t="s">
+        <v>135</v>
       </c>
       <c r="BB5" s="1" t="s">
         <v>41</v>
@@ -7004,30 +6985,30 @@
         <v>86</v>
       </c>
       <c r="M6" s="27"/>
-      <c r="AB6" s="34" t="s">
+      <c r="AB6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="AC6" s="40">
+      <c r="AC6" s="86">
         <v>2000</v>
       </c>
-      <c r="AD6" s="35">
+      <c r="AD6" s="58">
         <v>12</v>
       </c>
-      <c r="AE6" s="51">
+      <c r="AE6" s="87">
         <f>AC6 / AD6</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="AF6" s="35">
+      <c r="AF6" s="58">
         <v>100</v>
       </c>
-      <c r="AG6" s="52">
+      <c r="AG6" s="88">
         <f>AF6 * AD6</f>
         <v>1200</v>
       </c>
       <c r="AK6" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="AL6" s="42">
+        <v>121</v>
+      </c>
+      <c r="AL6" s="39">
         <f t="array" ref="AL6:AL8">TRANSPOSE(AC18:AE18)</f>
         <v>191.66666666666666</v>
       </c>
@@ -7038,7 +7019,7 @@
         <v>40</v>
       </c>
       <c r="AO6" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="AQ6" s="4" t="str">
         <f>_xlfn.TEXTJOIN(CHAR(9), FALSE, AK6,ROUND(AL6,2),AM6:AO6)</f>
@@ -7073,30 +7054,30 @@
       <c r="A7" s="3"/>
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
-      <c r="AB7" s="37" t="s">
+      <c r="AB7" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="AC7" s="41">
+      <c r="AC7" s="38">
         <v>1700</v>
       </c>
-      <c r="AD7" s="38">
+      <c r="AD7" s="36">
         <v>10</v>
       </c>
-      <c r="AE7" s="51">
+      <c r="AE7" s="42">
         <f>AC7 / AD7</f>
         <v>170</v>
       </c>
-      <c r="AF7" s="38">
+      <c r="AF7" s="36">
         <v>200</v>
       </c>
-      <c r="AG7" s="52">
+      <c r="AG7" s="43">
         <f>AF7 * AD7</f>
         <v>2000</v>
       </c>
       <c r="AK7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="AL7" s="42">
+        <v>139</v>
+      </c>
+      <c r="AL7" s="39">
         <v>187.5</v>
       </c>
       <c r="AM7" s="1" t="s">
@@ -7144,15 +7125,15 @@
       </c>
       <c r="M8" s="27"/>
       <c r="X8" s="1">
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="AB8" s="3"/>
       <c r="AC8" s="23"/>
       <c r="AI8" s="3"/>
       <c r="AK8" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="AL8" s="42">
+        <v>123</v>
+      </c>
+      <c r="AL8" s="39">
         <v>189.58333333333331</v>
       </c>
       <c r="AM8" s="1" t="s">
@@ -7201,17 +7182,17 @@
       <c r="T9" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="AB9" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="AC9" s="31"/>
-      <c r="AD9" s="31"/>
-      <c r="AE9" s="31"/>
+      <c r="AB9" s="85" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC9" s="85"/>
+      <c r="AD9" s="85"/>
+      <c r="AE9" s="85"/>
       <c r="AI9" s="3"/>
       <c r="AK9" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="AL9" s="42">
+        <v>122</v>
+      </c>
+      <c r="AL9" s="39">
         <f t="array" ref="AL9:AL11">TRANSPOSE(AC19:AE19)</f>
         <v>200</v>
       </c>
@@ -7255,21 +7236,21 @@
       <c r="E10" s="3"/>
       <c r="L10" s="27"/>
       <c r="M10" s="27"/>
-      <c r="AB10" s="43"/>
-      <c r="AC10" s="43" t="s">
+      <c r="AB10" s="94"/>
+      <c r="AC10" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD10" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="AD10" s="43" t="s">
+      <c r="AE10" s="94" t="s">
         <v>104</v>
-      </c>
-      <c r="AE10" s="43" t="s">
-        <v>105</v>
       </c>
       <c r="AI10" s="3"/>
       <c r="AK10" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="AL10" s="42">
+        <v>140</v>
+      </c>
+      <c r="AL10" s="39">
         <v>195</v>
       </c>
       <c r="AM10" s="1" t="s">
@@ -7318,22 +7299,22 @@
       <c r="K11" s="2"/>
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
-      <c r="AB11" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="AC11" s="44">
+      <c r="AB11" s="89" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC11" s="90">
         <v>300</v>
       </c>
-      <c r="AD11" s="45">
+      <c r="AD11" s="91">
         <v>250</v>
       </c>
-      <c r="AE11" s="46">
+      <c r="AE11" s="92">
         <v>275</v>
       </c>
       <c r="AK11" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="AL11" s="42">
+        <v>124</v>
+      </c>
+      <c r="AL11" s="39">
         <v>197.5</v>
       </c>
       <c r="AM11" s="1" t="s">
@@ -7384,13 +7365,13 @@
       <c r="T12" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="AB12" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="AC12" s="35"/>
-      <c r="AD12" s="35"/>
-      <c r="AE12" s="36"/>
-      <c r="AL12" s="42"/>
+      <c r="AB12" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC12" s="33"/>
+      <c r="AD12" s="33"/>
+      <c r="AE12" s="34"/>
+      <c r="AL12" s="39"/>
       <c r="AU12" s="4"/>
       <c r="BA12" t="s">
         <v>35</v>
@@ -7430,25 +7411,25 @@
         <v>87</v>
       </c>
       <c r="M13" s="27"/>
-      <c r="AB13" s="47" t="s">
+      <c r="AB13" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="AC13" s="53">
-        <f>AC$11 / $AD6</f>
+      <c r="AC13" s="44">
+        <f t="shared" ref="AC13:AE14" si="1">AC$11 / $AD6</f>
         <v>25</v>
       </c>
-      <c r="AD13" s="53">
-        <f>AD$11 / $AD6</f>
+      <c r="AD13" s="44">
+        <f t="shared" si="1"/>
         <v>20.833333333333332</v>
       </c>
-      <c r="AE13" s="54">
-        <f>AE$11 / $AD6</f>
+      <c r="AE13" s="45">
+        <f t="shared" si="1"/>
         <v>22.916666666666668</v>
       </c>
       <c r="AK13" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AL13" s="42">
+        <v>128</v>
+      </c>
+      <c r="AL13" s="39">
         <v>1</v>
       </c>
       <c r="AM13" s="1" t="s">
@@ -7459,7 +7440,7 @@
         <v>505</v>
       </c>
       <c r="AQ13" s="4" t="str">
-        <f t="shared" ref="AQ13:AQ18" si="1">_xlfn.TEXTJOIN(CHAR(9), FALSE, AK13,ROUND(AL13,2),AM13:AO13)</f>
+        <f t="shared" ref="AQ13:AQ18" si="2">_xlfn.TEXTJOIN(CHAR(9), FALSE, AK13,ROUND(AL13,2),AM13:AO13)</f>
         <v xml:space="preserve">[ScranMult, Scranton]	1	.	505	</v>
       </c>
       <c r="AU13" s="4"/>
@@ -7495,25 +7476,25 @@
       <c r="V14" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="AB14" s="37" t="s">
+      <c r="AB14" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="AC14" s="55">
-        <f>AC$11 / $AD7</f>
+      <c r="AC14" s="46">
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="AD14" s="55">
-        <f>AD$11 / $AD7</f>
+      <c r="AD14" s="46">
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="AE14" s="56">
-        <f>AE$11 / $AD7</f>
+      <c r="AE14" s="47">
+        <f t="shared" si="1"/>
         <v>27.5</v>
       </c>
       <c r="AK14" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="AL14" s="42">
+        <v>128</v>
+      </c>
+      <c r="AL14" s="39">
         <f>AE24</f>
         <v>1.5</v>
       </c>
@@ -7525,10 +7506,10 @@
         <v>100</v>
       </c>
       <c r="AO14" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AQ14" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>[ScranMult, Scranton]	1.5	.	100	# 1.5 multiplied if using overtime per plant</v>
       </c>
       <c r="AU14" s="4"/>
@@ -7564,9 +7545,9 @@
       </c>
       <c r="M15" s="27"/>
       <c r="AK15" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AL15" s="42">
+        <v>129</v>
+      </c>
+      <c r="AL15" s="39">
         <v>1</v>
       </c>
       <c r="AM15" s="1" t="s">
@@ -7577,7 +7558,7 @@
         <v>465</v>
       </c>
       <c r="AQ15" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">[UticaMult, Utica]	1	.	465	</v>
       </c>
       <c r="AU15" s="4"/>
@@ -7620,16 +7601,16 @@
       <c r="V16" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="AB16" s="59" t="s">
-        <v>151</v>
-      </c>
-      <c r="AC16" s="59"/>
-      <c r="AD16" s="59"/>
-      <c r="AE16" s="59"/>
+      <c r="AB16" s="31" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="31"/>
+      <c r="AE16" s="31"/>
       <c r="AK16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="AL16" s="42">
+        <v>129</v>
+      </c>
+      <c r="AL16" s="39">
         <f>AE25</f>
         <v>1.5</v>
       </c>
@@ -7641,7 +7622,7 @@
         <v>100</v>
       </c>
       <c r="AQ16" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">[UticaMult, Utica]	1.5	.	100	</v>
       </c>
       <c r="AU16" s="4"/>
@@ -7674,32 +7655,32 @@
       <c r="A17" s="3"/>
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
-      <c r="AB17" s="67"/>
-      <c r="AC17" s="67" t="s">
+      <c r="AB17" s="95"/>
+      <c r="AC17" s="95" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD17" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="AD17" s="67" t="s">
+      <c r="AE17" s="95" t="s">
         <v>104</v>
       </c>
-      <c r="AE17" s="67" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF17" s="72" t="str">
-        <f t="shared" ref="AF17:AH17" si="2">AC17</f>
+      <c r="AF17" s="61" t="str">
+        <f t="shared" ref="AF17:AH17" si="3">AC17</f>
         <v>Scranton, PA</v>
       </c>
-      <c r="AG17" s="72" t="str">
-        <f t="shared" si="2"/>
+      <c r="AG17" s="61" t="str">
+        <f t="shared" si="3"/>
         <v>Utica, NY</v>
       </c>
-      <c r="AH17" s="72" t="str">
-        <f t="shared" si="2"/>
+      <c r="AH17" s="61" t="str">
+        <f t="shared" si="3"/>
         <v>Stamford, CT</v>
       </c>
       <c r="AK17" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AL17" s="42">
+        <v>130</v>
+      </c>
+      <c r="AL17" s="39">
         <v>1</v>
       </c>
       <c r="AM17" s="1" t="s">
@@ -7710,7 +7691,7 @@
         <v>570</v>
       </c>
       <c r="AQ17" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">[StamMult, Stamford]	1	.	570	</v>
       </c>
       <c r="AU17" s="4"/>
@@ -7746,37 +7727,37 @@
       <c r="U18" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AB18" s="58" t="s">
+      <c r="AB18" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="AC18" s="60">
-        <f>AC13 + $AE6</f>
+      <c r="AC18" s="50">
+        <f t="shared" ref="AC18:AE19" si="4">AC13 + $AE6</f>
         <v>191.66666666666666</v>
       </c>
-      <c r="AD18" s="60">
-        <f>AD13 + $AE6</f>
+      <c r="AD18" s="50">
+        <f t="shared" si="4"/>
         <v>187.5</v>
       </c>
-      <c r="AE18" s="61">
-        <f>AE13 + $AE6</f>
+      <c r="AE18" s="51">
+        <f t="shared" si="4"/>
         <v>189.58333333333331</v>
       </c>
-      <c r="AF18" s="72" t="str">
+      <c r="AF18" s="61" t="str">
         <f>"(" &amp; TEXT(AC18, "#,##0.00") &amp; ",0,∞)"</f>
         <v>(191.67,0,∞)</v>
       </c>
-      <c r="AG18" s="72" t="str">
-        <f t="shared" ref="AG18:AG19" si="3">"(" &amp; TEXT(AD18, "#,##0.00") &amp; ",0,∞)"</f>
+      <c r="AG18" s="61" t="str">
+        <f t="shared" ref="AG18:AG19" si="5">"(" &amp; TEXT(AD18, "#,##0.00") &amp; ",0,∞)"</f>
         <v>(187.50,0,∞)</v>
       </c>
-      <c r="AH18" s="72" t="str">
-        <f t="shared" ref="AH18:AH19" si="4">"(" &amp; TEXT(AE18, "#,##0.00") &amp; ",0,∞)"</f>
+      <c r="AH18" s="61" t="str">
+        <f t="shared" ref="AH18:AH19" si="6">"(" &amp; TEXT(AE18, "#,##0.00") &amp; ",0,∞)"</f>
         <v>(189.58,0,∞)</v>
       </c>
       <c r="AK18" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="AL18" s="42">
+        <v>130</v>
+      </c>
+      <c r="AL18" s="39">
         <f>AE26</f>
         <v>1.5</v>
       </c>
@@ -7788,7 +7769,7 @@
         <v>100</v>
       </c>
       <c r="AQ18" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v xml:space="preserve">[StamMult, Stamford]	1.5	.	100	</v>
       </c>
     </row>
@@ -7808,34 +7789,34 @@
       <c r="O19" s="1">
         <v>0</v>
       </c>
-      <c r="AB19" s="57" t="s">
+      <c r="AB19" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="AC19" s="62">
-        <f>AC14 + $AE7</f>
+      <c r="AC19" s="52">
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
-      <c r="AD19" s="62">
-        <f>AD14 + $AE7</f>
+      <c r="AD19" s="52">
+        <f t="shared" si="4"/>
         <v>195</v>
       </c>
-      <c r="AE19" s="63">
-        <f>AE14 + $AE7</f>
+      <c r="AE19" s="53">
+        <f t="shared" si="4"/>
         <v>197.5</v>
       </c>
-      <c r="AF19" s="72" t="str">
-        <f t="shared" ref="AF19" si="5">"(" &amp; TEXT(AC19, "#,##0.00") &amp; ",0,∞)"</f>
+      <c r="AF19" s="61" t="str">
+        <f t="shared" ref="AF19" si="7">"(" &amp; TEXT(AC19, "#,##0.00") &amp; ",0,∞)"</f>
         <v>(200.00,0,∞)</v>
       </c>
-      <c r="AG19" s="72" t="str">
-        <f t="shared" si="3"/>
+      <c r="AG19" s="61" t="str">
+        <f t="shared" si="5"/>
         <v>(195.00,0,∞)</v>
       </c>
-      <c r="AH19" s="72" t="str">
-        <f t="shared" si="4"/>
+      <c r="AH19" s="61" t="str">
+        <f t="shared" si="6"/>
         <v>(197.50,0,∞)</v>
       </c>
-      <c r="AL19" s="42"/>
+      <c r="AL19" s="39"/>
     </row>
     <row r="20" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
@@ -7847,9 +7828,9 @@
         <v>90</v>
       </c>
       <c r="AK20" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="AL20" s="42">
+        <v>136</v>
+      </c>
+      <c r="AL20" s="39">
         <f t="array" ref="AL20:AL21">TRANSPOSE(AG31:AH31)</f>
         <v>98</v>
       </c>
@@ -7860,10 +7841,10 @@
         <v>40</v>
       </c>
       <c r="AO20" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="AQ20" s="4" t="str">
-        <f t="shared" ref="AQ20:AQ29" si="6">_xlfn.TEXTJOIN(CHAR(9), FALSE, AK20,ROUND(AL20,2),AM20:AO20)</f>
+        <f t="shared" ref="AQ20:AQ28" si="8">_xlfn.TEXTJOIN(CHAR(9), FALSE, AK20,ROUND(AL20,2),AM20:AO20)</f>
         <v>[Scranton,   Goggle]	98	.	.	# Cost of manufacturing + transportation to businesses (See calcs in screenshot)</v>
       </c>
     </row>
@@ -7876,9 +7857,9 @@
       <c r="L21" s="27"/>
       <c r="M21" s="27"/>
       <c r="AK21" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="AL21" s="91">
+        <v>118</v>
+      </c>
+      <c r="AL21" s="78">
         <v>105</v>
       </c>
       <c r="AM21" s="6" t="s">
@@ -7888,7 +7869,7 @@
         <v>40</v>
       </c>
       <c r="AQ21" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">[Scranton,   Faceblock]	105	.	.	</v>
       </c>
     </row>
@@ -7909,17 +7890,17 @@
       <c r="X22" s="1">
         <v>-600</v>
       </c>
-      <c r="AB22" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="AC22" s="64"/>
-      <c r="AD22" s="64"/>
-      <c r="AE22" s="64"/>
+      <c r="AB22" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC22" s="54"/>
+      <c r="AD22" s="54"/>
+      <c r="AE22" s="54"/>
       <c r="AK22" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="AL22" s="42">
-        <v>1000</v>
+        <v>131</v>
+      </c>
+      <c r="AL22" s="39">
+        <v>0</v>
       </c>
       <c r="AM22" s="1" t="s">
         <v>40</v>
@@ -7928,8 +7909,8 @@
         <v>40</v>
       </c>
       <c r="AQ22" s="4" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">[Scranton,   dummy  ]	1000	.	.	</v>
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">[Scranton,   dummy  ]	0	.	.	</v>
       </c>
     </row>
     <row r="23" spans="1:62" x14ac:dyDescent="0.3">
@@ -7942,23 +7923,23 @@
       <c r="S23" s="28"/>
       <c r="U23" s="30"/>
       <c r="V23" s="28" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="W23" s="27"/>
-      <c r="AB23" s="71"/>
-      <c r="AC23" s="71" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD23" s="71" t="s">
+      <c r="AB23" s="60"/>
+      <c r="AC23" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD23" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="AE23" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="AE23" s="71" t="s">
-        <v>112</v>
-      </c>
       <c r="AK23" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="AL23" s="42">
+        <v>137</v>
+      </c>
+      <c r="AL23" s="39">
         <f t="array" ref="AL23:AL24">TRANSPOSE(AG32:AH32)</f>
         <v>119</v>
       </c>
@@ -7969,7 +7950,7 @@
         <v>40</v>
       </c>
       <c r="AQ23" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">[Utica,      Goggle]	119	.	.	</v>
       </c>
       <c r="BJ23" s="23" t="s">
@@ -7983,27 +7964,27 @@
       <c r="Q24" s="29"/>
       <c r="R24" s="28"/>
       <c r="S24" s="30" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="T24" s="30"/>
       <c r="U24" s="30"/>
       <c r="V24" s="30"/>
-      <c r="AB24" s="68" t="s">
+      <c r="AB24" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="AC24" s="69">
+      <c r="AC24" s="58">
         <v>505</v>
       </c>
-      <c r="AD24" s="70">
+      <c r="AD24" s="59">
         <v>100</v>
       </c>
-      <c r="AE24" s="70">
+      <c r="AE24" s="59">
         <v>1.5</v>
       </c>
       <c r="AK24" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL24" s="42">
+        <v>119</v>
+      </c>
+      <c r="AL24" s="39">
         <v>123</v>
       </c>
       <c r="AM24" s="1" t="s">
@@ -8013,7 +7994,7 @@
         <v>40</v>
       </c>
       <c r="AQ24" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">[Utica,      Faceblock]	123	.	.	</v>
       </c>
       <c r="BJ24" s="23" t="s">
@@ -8026,31 +8007,31 @@
       <c r="M25" s="27"/>
       <c r="Q25" s="29"/>
       <c r="S25" s="30" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="T25" s="28"/>
       <c r="U25" s="28"/>
       <c r="V25" s="28"/>
-      <c r="AB25" s="47" t="s">
+      <c r="AB25" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="AC25" s="65">
+      <c r="AC25" s="55">
         <v>465</v>
       </c>
-      <c r="AD25" s="66">
-        <f t="shared" ref="AD25:AE26" si="7">AD24</f>
+      <c r="AD25" s="56">
+        <f t="shared" ref="AD25:AE26" si="9">AD24</f>
         <v>100</v>
       </c>
-      <c r="AE25" s="66">
-        <f t="shared" si="7"/>
+      <c r="AE25" s="56">
+        <f t="shared" si="9"/>
         <v>1.5</v>
       </c>
       <c r="AK25" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="AL25" s="42">
+        <v>132</v>
+      </c>
+      <c r="AL25" s="39">
         <f>AL$22</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM25" s="1" t="s">
         <v>40</v>
@@ -8059,36 +8040,39 @@
         <v>40</v>
       </c>
       <c r="AQ25" s="4" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">[Utica,      dummy   ]	1000	.	.	</v>
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">[Utica,      dummy   ]	0	.	.	</v>
       </c>
     </row>
     <row r="26" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
+      <c r="I26" s="82" t="s">
+        <v>154</v>
+      </c>
       <c r="Q26" s="29"/>
       <c r="R26" s="28"/>
       <c r="S26" s="28"/>
       <c r="T26" s="28"/>
       <c r="U26" s="28"/>
       <c r="V26" s="28"/>
-      <c r="AB26" s="37" t="s">
+      <c r="AB26" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="AC26" s="38">
+      <c r="AC26" s="36">
         <v>570</v>
       </c>
-      <c r="AD26" s="39">
-        <f t="shared" si="7"/>
+      <c r="AD26" s="37">
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
-      <c r="AE26" s="39">
-        <f t="shared" si="7"/>
+      <c r="AE26" s="37">
+        <f t="shared" si="9"/>
         <v>1.5</v>
       </c>
       <c r="AK26" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="AL26" s="42">
+        <v>138</v>
+      </c>
+      <c r="AL26" s="39">
         <f t="array" ref="AL26:AL27">TRANSPOSE(AG33:AH33)</f>
         <v>139</v>
       </c>
@@ -8099,7 +8083,7 @@
         <v>40</v>
       </c>
       <c r="AQ26" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">[Stamford,   Goggle]	139	.	.	</v>
       </c>
     </row>
@@ -8113,9 +8097,9 @@
       <c r="AH27" s="1"/>
       <c r="AJ27" s="2"/>
       <c r="AK27" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AL27" s="42">
+        <v>120</v>
+      </c>
+      <c r="AL27" s="39">
         <v>135</v>
       </c>
       <c r="AM27" s="1" t="s">
@@ -8126,11 +8110,11 @@
       </c>
       <c r="AO27" s="18"/>
       <c r="AQ27" s="4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v xml:space="preserve">[Stamford,   Faceblock]	135	.	.	</v>
       </c>
-      <c r="AR27" s="89"/>
-      <c r="AS27" s="89"/>
+      <c r="AR27" s="76"/>
+      <c r="AS27" s="76"/>
       <c r="BG27" s="18"/>
     </row>
     <row r="28" spans="1:62" x14ac:dyDescent="0.3">
@@ -8142,11 +8126,11 @@
       <c r="AG28" s="6"/>
       <c r="AH28" s="6"/>
       <c r="AK28" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="AL28" s="42">
+        <v>134</v>
+      </c>
+      <c r="AL28" s="39">
         <f>AL$22</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="AM28" s="1" t="s">
         <v>40</v>
@@ -8155,27 +8139,27 @@
         <v>40</v>
       </c>
       <c r="AQ28" s="4" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">[Stamford,   dummy   ]	1000	.	.	</v>
+        <f t="shared" si="8"/>
+        <v xml:space="preserve">[Stamford,   dummy   ]	0	.	.	</v>
       </c>
     </row>
     <row r="29" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="B29" s="85" t="s">
+      <c r="B29" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="86"/>
-      <c r="AB29" s="73" t="s">
+      <c r="C29" s="73"/>
+      <c r="AB29" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC29" s="83"/>
+      <c r="AD29" s="83"/>
+      <c r="AE29" s="83"/>
+      <c r="AG29" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="AC29" s="73"/>
-      <c r="AD29" s="73"/>
-      <c r="AE29" s="73"/>
-      <c r="AG29" s="73" t="s">
-        <v>117</v>
-      </c>
-      <c r="AH29" s="73"/>
+      <c r="AH29" s="83"/>
       <c r="AK29" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AQ29" s="4" t="str">
         <f>_xlfn.TEXTJOIN(CHAR(9), FALSE, AK29,AL29,AM29:AO29)</f>
@@ -8183,92 +8167,92 @@
       </c>
     </row>
     <row r="30" spans="1:62" ht="21" x14ac:dyDescent="0.35">
-      <c r="B30" s="85" t="s">
-        <v>96</v>
-      </c>
-      <c r="C30" s="87"/>
+      <c r="B30" s="72" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="74"/>
       <c r="X30" s="1">
         <v>-1600</v>
       </c>
-      <c r="AB30" s="77"/>
-      <c r="AC30" s="77" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD30" s="77" t="s">
+      <c r="AB30" s="84"/>
+      <c r="AC30" s="84" t="s">
+        <v>114</v>
+      </c>
+      <c r="AD30" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE30" s="84" t="s">
         <v>113</v>
       </c>
-      <c r="AE30" s="77" t="s">
-        <v>114</v>
-      </c>
-      <c r="AG30" s="77" t="str">
+      <c r="AG30" s="84" t="str">
         <f>AD30</f>
         <v>Goggle</v>
       </c>
-      <c r="AH30" s="77" t="str">
+      <c r="AH30" s="84" t="str">
         <f>AE30</f>
         <v>Faceblock</v>
       </c>
     </row>
     <row r="31" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="AB31" s="76" t="str">
+      <c r="AB31" s="64" t="str">
         <f>AB24</f>
         <v>Scranton</v>
       </c>
-      <c r="AC31" s="78">
+      <c r="AC31" s="65">
         <v>90</v>
       </c>
-      <c r="AD31" s="78">
+      <c r="AD31" s="65">
         <v>8</v>
       </c>
-      <c r="AE31" s="79">
+      <c r="AE31" s="66">
         <v>15</v>
       </c>
-      <c r="AG31" s="78">
-        <f>$AC31 + AD31</f>
+      <c r="AG31" s="65">
+        <f t="shared" ref="AG31:AH33" si="10">$AC31 + AD31</f>
         <v>98</v>
       </c>
-      <c r="AH31" s="79">
-        <f>$AC31 + AE31</f>
+      <c r="AH31" s="66">
+        <f t="shared" si="10"/>
         <v>105</v>
       </c>
       <c r="AK31" s="32"/>
       <c r="AL31" s="32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AO31" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AR31" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AS31" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:62" x14ac:dyDescent="0.3">
-      <c r="AB32" s="74" t="str">
+      <c r="AB32" s="62" t="str">
         <f>AB25</f>
         <v>Utica</v>
       </c>
-      <c r="AC32" s="80">
+      <c r="AC32" s="67">
         <v>105</v>
       </c>
-      <c r="AD32" s="80">
+      <c r="AD32" s="67">
         <v>14</v>
       </c>
-      <c r="AE32" s="81">
+      <c r="AE32" s="68">
         <v>18</v>
       </c>
-      <c r="AG32" s="80">
-        <f>$AC32 + AD32</f>
+      <c r="AG32" s="67">
+        <f t="shared" si="10"/>
         <v>119</v>
       </c>
-      <c r="AH32" s="81">
-        <f>$AC32 + AE32</f>
+      <c r="AH32" s="68">
+        <f t="shared" si="10"/>
         <v>123</v>
       </c>
       <c r="AK32" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="AQ32" s="4" t="str">
         <f>_xlfn.TEXTJOIN(CHAR(9), FALSE, AK32,AL32,AM32:AO32)</f>
@@ -8276,36 +8260,36 @@
       </c>
     </row>
     <row r="33" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="AB33" s="75" t="str">
+      <c r="AB33" s="63" t="str">
         <f>AB26</f>
         <v>Stamford</v>
       </c>
-      <c r="AC33" s="82">
+      <c r="AC33" s="69">
         <v>115</v>
       </c>
-      <c r="AD33" s="82">
+      <c r="AD33" s="69">
         <v>24</v>
       </c>
-      <c r="AE33" s="83">
+      <c r="AE33" s="70">
         <v>20</v>
       </c>
-      <c r="AG33" s="82">
-        <f>$AC33 + AD33</f>
+      <c r="AG33" s="69">
+        <f t="shared" si="10"/>
         <v>139</v>
       </c>
-      <c r="AH33" s="83">
-        <f>$AC33 + AE33</f>
+      <c r="AH33" s="70">
+        <f t="shared" si="10"/>
         <v>135</v>
       </c>
       <c r="AK33" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AL33" s="92">
+      <c r="AL33" s="79">
         <f>AG6</f>
         <v>1200</v>
       </c>
-      <c r="AM33" s="93" t="s">
-        <v>145</v>
+      <c r="AM33" s="80" t="s">
+        <v>143</v>
       </c>
       <c r="AQ33" s="4" t="str">
         <f>_xlfn.TEXTJOIN(CHAR(9), FALSE, AK33,AL33,AM33:AO33)</f>
@@ -8316,15 +8300,15 @@
       <c r="AK34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AL34" s="92">
+      <c r="AL34" s="79">
         <f>AG7</f>
         <v>2000</v>
       </c>
-      <c r="AM34" s="93" t="s">
-        <v>146</v>
+      <c r="AM34" s="80" t="s">
+        <v>144</v>
       </c>
       <c r="AQ34" s="4" t="str">
-        <f t="shared" ref="AQ34:AQ46" si="8">_xlfn.TEXTJOIN(CHAR(9), FALSE, AK34,AL34,AM34:AO34)</f>
+        <f t="shared" ref="AQ34:AQ46" si="11">_xlfn.TEXTJOIN(CHAR(9), FALSE, AK34,AL34,AM34:AO34)</f>
         <v xml:space="preserve">Generalist	2000	# 10 units * 200 labor hours		</v>
       </c>
     </row>
@@ -8332,10 +8316,10 @@
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="AK35" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="AQ35" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"># Transshippment (Plants or OT Multiplier)				</v>
       </c>
     </row>
@@ -8343,13 +8327,13 @@
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="AK36" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AL36" s="1">
         <v>0</v>
       </c>
       <c r="AQ36" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">ScranMult	0			</v>
       </c>
     </row>
@@ -8357,13 +8341,13 @@
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="AK37" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AL37" s="1">
         <v>0</v>
       </c>
       <c r="AQ37" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">UticaMult	0			</v>
       </c>
     </row>
@@ -8371,13 +8355,13 @@
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="AK38" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AL38" s="1">
         <v>0</v>
       </c>
       <c r="AQ38" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">StamMult	0			</v>
       </c>
     </row>
@@ -8395,7 +8379,7 @@
         <v>0</v>
       </c>
       <c r="AQ39" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">Scranton	0			</v>
       </c>
     </row>
@@ -8413,7 +8397,7 @@
         <v>0</v>
       </c>
       <c r="AQ40" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">Utica	0			</v>
       </c>
     </row>
@@ -8431,7 +8415,7 @@
         <v>0</v>
       </c>
       <c r="AQ41" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">Stamford	0			</v>
       </c>
     </row>
@@ -8443,10 +8427,10 @@
         <v>48</v>
       </c>
       <c r="AK42" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="AQ42" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve"># Demand				</v>
       </c>
     </row>
@@ -8454,15 +8438,15 @@
       <c r="C43" s="8"/>
       <c r="D43" s="23"/>
       <c r="AK43" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AL43" s="1">
         <f>X8</f>
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="AQ43" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">Goggle	-1000			</v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">Goggle	0			</v>
       </c>
     </row>
     <row r="44" spans="1:43" ht="20.25" x14ac:dyDescent="0.35">
@@ -8473,32 +8457,32 @@
         <v>9</v>
       </c>
       <c r="AK44" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AL44" s="1">
         <f>X22</f>
         <v>-600</v>
       </c>
-      <c r="AM44" s="93" t="s">
-        <v>148</v>
+      <c r="AM44" s="80" t="s">
+        <v>157</v>
       </c>
       <c r="AQ44" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">Faceblock	-600	# 1200 + 2000 - 1000 - 600		</v>
+        <f t="shared" si="11"/>
+        <v xml:space="preserve">Faceblock	-600	# 1200 + 2000 - 0 - 600		</v>
       </c>
     </row>
     <row r="45" spans="1:43" x14ac:dyDescent="0.3">
       <c r="C45" s="8"/>
       <c r="D45" s="23"/>
       <c r="AK45" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AL45" s="1">
         <f>X30</f>
         <v>-1600</v>
       </c>
       <c r="AQ45" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">dummy	-1600			</v>
       </c>
     </row>
@@ -8510,10 +8494,10 @@
         <v>11</v>
       </c>
       <c r="AK46" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AQ46" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v xml:space="preserve">;				</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Problem 3 and 4 FINISHED!
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 02/Network Flow Graphs.xlsx
+++ b/03 - Homework/HW 02/Network Flow Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chickasawnation-my.sharepoint.com/personal/daniel_carpenter_chickasaw_net/Documents/Documents/GitHub/OU-DSA/Metaheuristics/03 - Homework/HW 02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2791" documentId="8_{DDE69595-AFB4-4123-BB98-2CC2CEAC48BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{08E6820F-A08E-4240-944C-19E245FD2216}"/>
+  <xr:revisionPtr revIDLastSave="2806" documentId="8_{DDE69595-AFB4-4123-BB98-2CC2CEAC48BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{200A3365-6053-49D6-A9CD-904151679AC3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
+    <workbookView minimized="1" xWindow="6060" yWindow="795" windowWidth="15075" windowHeight="14805" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE14DA27-A8C1-45F9-9C11-8787018CF8AD}"/>
   </bookViews>
   <sheets>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="190">
   <si>
     <t>Labor Sources</t>
   </si>
@@ -1104,6 +1104,9 @@
       <t>(d)</t>
     </r>
   </si>
+  <si>
+    <t>A</t>
+  </si>
 </sst>
 </file>
 
@@ -1117,7 +1120,7 @@
     <numFmt numFmtId="166" formatCode="&quot;(&quot;0&quot;)&quot;"/>
     <numFmt numFmtId="167" formatCode="&quot;(&quot;0&quot;,0,∞)&quot;"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1353,6 +1356,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1422,7 +1432,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -1895,12 +1905,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2256,8 +2288,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2305,8 +2344,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2125755" y="2765051"/>
-          <a:ext cx="1281219" cy="3682230"/>
+          <a:off x="2125755" y="2854698"/>
+          <a:ext cx="1281219" cy="3682231"/>
           <a:chOff x="3321050" y="1548093"/>
           <a:chExt cx="1281219" cy="3682230"/>
         </a:xfrm>
@@ -2527,7 +2566,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5013137" y="2765051"/>
+          <a:off x="5013137" y="2854698"/>
           <a:ext cx="2475391" cy="3659820"/>
           <a:chOff x="5013137" y="1543610"/>
           <a:chExt cx="2475391" cy="3659820"/>
@@ -2860,7 +2899,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8901953" y="2765051"/>
+          <a:off x="8901953" y="2854698"/>
           <a:ext cx="3680769" cy="3659820"/>
           <a:chOff x="3807759" y="1543610"/>
           <a:chExt cx="3680769" cy="3659820"/>
@@ -3365,7 +3404,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="14085794" y="2765051"/>
+          <a:off x="14085794" y="2854698"/>
           <a:ext cx="3714386" cy="3659820"/>
           <a:chOff x="3807759" y="1543610"/>
           <a:chExt cx="3680769" cy="3659820"/>
@@ -10151,8 +10190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F6EB8B-EEA2-48C7-A135-DB48C73C0E00}">
   <dimension ref="B2:AK34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1"/>
   </sheetViews>
@@ -10175,36 +10214,46 @@
     <col min="38" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:37" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="70" t="s">
+    <row r="2" spans="2:37" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B2"/>
+      <c r="C2" s="143" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="143"/>
-      <c r="I2" s="70" t="s">
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="143"/>
+      <c r="G2"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="143" t="s">
         <v>177</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="P2" s="70" t="s">
+      <c r="J2" s="143"/>
+      <c r="K2" s="143"/>
+      <c r="L2" s="143"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="144"/>
+      <c r="O2" s="144"/>
+      <c r="P2" s="143" t="s">
         <v>178</v>
       </c>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="X2" s="70" t="s">
+      <c r="Q2" s="143"/>
+      <c r="R2" s="143"/>
+      <c r="S2" s="143"/>
+      <c r="T2" s="143"/>
+      <c r="U2" s="144"/>
+      <c r="V2" s="144"/>
+      <c r="W2" s="144"/>
+      <c r="X2" s="143" t="s">
         <v>179</v>
       </c>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="70"/>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="70"/>
+      <c r="Y2" s="143"/>
+      <c r="Z2" s="143"/>
+      <c r="AA2" s="143"/>
+      <c r="AB2" s="143"/>
+      <c r="AC2" s="143"/>
+    </row>
+    <row r="3" spans="2:37" x14ac:dyDescent="0.3">
+      <c r="G3"/>
     </row>
     <row r="4" spans="2:37" x14ac:dyDescent="0.3">
       <c r="AG4" s="31" t="s">
@@ -10598,7 +10647,7 @@
       <c r="AB16" s="113"/>
       <c r="AC16" s="113"/>
     </row>
-    <row r="17" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D17" s="113"/>
       <c r="E17" s="117">
         <v>600</v>
@@ -10632,7 +10681,7 @@
       <c r="AB17" s="113"/>
       <c r="AC17" s="113"/>
     </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D18" s="113"/>
       <c r="E18" s="113"/>
       <c r="F18" s="113"/>
@@ -10662,7 +10711,7 @@
       <c r="AB18" s="113"/>
       <c r="AC18" s="113"/>
     </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D19" s="113"/>
       <c r="E19" s="113"/>
       <c r="F19" s="113"/>
@@ -10698,7 +10747,7 @@
       </c>
       <c r="AC19" s="117"/>
     </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D20" s="116"/>
       <c r="E20" s="113"/>
       <c r="F20" s="113"/>
@@ -10728,7 +10777,7 @@
       </c>
       <c r="AD20" s="27"/>
     </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D21" s="113"/>
       <c r="E21" s="113"/>
       <c r="F21" s="113"/>
@@ -10760,7 +10809,7 @@
       <c r="AE21" s="113"/>
       <c r="AF21" s="113"/>
     </row>
-    <row r="22" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D22" s="113"/>
       <c r="E22" s="113"/>
       <c r="F22" s="113"/>
@@ -10787,7 +10836,7 @@
       <c r="AB22" s="113"/>
       <c r="AC22" s="113"/>
     </row>
-    <row r="23" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D23" s="113"/>
       <c r="E23" s="113"/>
       <c r="F23" s="113"/>
@@ -10824,7 +10873,7 @@
       <c r="AE23" s="27"/>
       <c r="AF23" s="27"/>
     </row>
-    <row r="24" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D24" s="112"/>
       <c r="E24" s="112"/>
       <c r="F24" s="112"/>
@@ -10855,7 +10904,7 @@
       <c r="AE24" s="112"/>
       <c r="AF24" s="112"/>
     </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D25" s="112"/>
       <c r="E25" s="23">
         <v>-320</v>
@@ -10895,7 +10944,7 @@
       </c>
       <c r="AD25" s="124"/>
     </row>
-    <row r="26" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:33" x14ac:dyDescent="0.3">
       <c r="D26" s="112"/>
       <c r="F26" s="112"/>
       <c r="G26" s="112"/>
@@ -10922,10 +10971,13 @@
       <c r="AE26" s="112"/>
       <c r="AF26" s="112"/>
     </row>
-    <row r="27" spans="2:32" x14ac:dyDescent="0.3">
-      <c r="D27" s="112"/>
-      <c r="E27" s="112"/>
-      <c r="F27" s="112"/>
+    <row r="27" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="C27" s="145" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="104"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="106"/>
       <c r="G27" s="112"/>
       <c r="H27" s="112"/>
       <c r="I27" s="112"/>
@@ -10957,7 +11009,13 @@
       <c r="AE27" s="112"/>
       <c r="AF27" s="112"/>
     </row>
-    <row r="28" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="C28" s="146" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" s="107"/>
+      <c r="E28" s="108"/>
+      <c r="F28" s="109"/>
       <c r="L28" s="112"/>
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
@@ -10980,7 +11038,7 @@
       <c r="AE28" s="112"/>
       <c r="AF28" s="112"/>
     </row>
-    <row r="29" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -11003,7 +11061,7 @@
       <c r="AB29" s="112"/>
       <c r="AC29" s="112"/>
     </row>
-    <row r="30" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
@@ -11026,7 +11084,7 @@
       <c r="AB30" s="112"/>
       <c r="AC30" s="112"/>
     </row>
-    <row r="31" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
@@ -11049,7 +11107,7 @@
       <c r="AB31" s="112"/>
       <c r="AC31" s="112"/>
     </row>
-    <row r="32" spans="2:32" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:33" x14ac:dyDescent="0.3">
       <c r="B32"/>
       <c r="C32"/>
       <c r="D32"/>
@@ -11071,6 +11129,9 @@
       <c r="AA32" s="112"/>
       <c r="AB32" s="112"/>
       <c r="AC32" s="112"/>
+      <c r="AG32" s="23" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="33" spans="2:29" x14ac:dyDescent="0.3">
       <c r="B33"/>
@@ -11119,7 +11180,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC69D54E-00BB-4469-9873-ACE66827EA4B}">
   <dimension ref="A1:BJ52"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D34" sqref="A34:D35"/>
+    </sheetView>
     <sheetView showGridLines="0" zoomScale="81" zoomScaleNormal="81" workbookViewId="1">
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
@@ -12896,9 +12959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599F1D43-9BD8-4A09-A61C-254B47A47DFE}">
   <dimension ref="B1:K22"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13290,9 +13351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70FBFC5-285A-4C09-B287-071ADBFF8F1F}">
   <dimension ref="B1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="W9" sqref="N1:W9"/>
-    </sheetView>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Scratch for problem 1
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 02/Network Flow Graphs.xlsx
+++ b/03 - Homework/HW 02/Network Flow Graphs.xlsx
@@ -5,20 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://chickasawnation-my.sharepoint.com/personal/daniel_carpenter_chickasaw_net/Documents/Documents/GitHub/OU-DSA/Metaheuristics/03 - Homework/HW 02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.carpenter\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2806" documentId="8_{DDE69595-AFB4-4123-BB98-2CC2CEAC48BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{200A3365-6053-49D6-A9CD-904151679AC3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80FFF920-F72B-4BFB-A688-D0590BC528E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6060" yWindow="795" windowWidth="15075" windowHeight="14805" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FE14DA27-A8C1-45F9-9C11-8787018CF8AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Problem 3" sheetId="4" r:id="rId1"/>
-    <sheet name="Problem 4" sheetId="2" r:id="rId2"/>
-    <sheet name="P4 Scratch" sheetId="3" r:id="rId3"/>
-    <sheet name="P3 Scratch" sheetId="5" r:id="rId4"/>
-    <sheet name="P4 V1" sheetId="1" state="hidden" r:id="rId5"/>
+    <sheet name="Problem 1(b) Scratch" sheetId="6" r:id="rId1"/>
+    <sheet name="Problem 3" sheetId="4" r:id="rId2"/>
+    <sheet name="Problem 4" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId5"/>
+    <sheet name="P4 Scratch" sheetId="3" state="hidden" r:id="rId6"/>
+    <sheet name="P3 Scratch" sheetId="5" state="hidden" r:id="rId7"/>
+    <sheet name="P4 V1" sheetId="1" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -38,8 +40,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="240">
   <si>
     <t>Labor Sources</t>
   </si>
@@ -1107,20 +1131,172 @@
   <si>
     <t>A</t>
   </si>
+  <si>
+    <t>Raisins</t>
+  </si>
+  <si>
+    <t>Juice</t>
+  </si>
+  <si>
+    <t>Jelly</t>
+  </si>
+  <si>
+    <t>Pounds per Product</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Tons of Product</t>
+  </si>
+  <si>
+    <t>Grade B</t>
+  </si>
+  <si>
+    <t>Grade A</t>
+  </si>
+  <si>
+    <t>% Contribution</t>
+  </si>
+  <si>
+    <t>Avg Points</t>
+  </si>
+  <si>
+    <t>Min Points</t>
+  </si>
+  <si>
+    <t>Raisin</t>
+  </si>
+  <si>
+    <t>Total Grade B Available</t>
+  </si>
+  <si>
+    <t>Total Raisins Calculated</t>
+  </si>
+  <si>
+    <t>% Grade B Used Towards Raisins, i.e. tier 8</t>
+  </si>
+  <si>
+    <t>Weighted Avg Cost per Pound</t>
+  </si>
+  <si>
+    <t>Weighted Avg. Cost per Pound</t>
+  </si>
+  <si>
+    <t>% Breakdown of Grades</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Cost per Pound</t>
+  </si>
+  <si>
+    <t>Fruit Cost (Pounds * Wt. Avg. Cost)</t>
+  </si>
+  <si>
+    <t>For raisins, this implies that 25% of the raisin production will stem from Grade B (and 75% towards A)</t>
+  </si>
+  <si>
+    <t>For juice, this implies that 75% of the juice production will stem from Grade B (and 25% towards A)</t>
+  </si>
+  <si>
+    <t>Note 100% Grade B used for Jelly.</t>
+  </si>
+  <si>
+    <t>&lt;- this is from the aboves assumptions text</t>
+  </si>
+  <si>
+    <t>&lt;- Noted in Table 2 footer</t>
+  </si>
+  <si>
+    <t>&lt;- noted in table 3 bullet 4</t>
+  </si>
+  <si>
+    <t>&lt;- 1 minus above</t>
+  </si>
+  <si>
+    <t>&lt;- this is how they determine the fruit cost in Table 3</t>
+  </si>
+  <si>
+    <t>Interpretation and Assumptions:</t>
+  </si>
+  <si>
+    <t>Problem 1 (a): Calculating the Upper Bound for the Raisin Product</t>
+  </si>
+  <si>
+    <t>Problem 1(b): Calculate the Fruit Cost seen in Table 3</t>
+  </si>
+  <si>
+    <t>&lt;- note this is the % towards A</t>
+  </si>
+  <si>
+    <t>&lt;- "" B</t>
+  </si>
+  <si>
+    <t>Less Raisin Dedicated Portion to Grade A</t>
+  </si>
+  <si>
+    <t>Grade B Portion Implied*</t>
+  </si>
+  <si>
+    <t>Supply</t>
+  </si>
+  <si>
+    <t>Decision Variables</t>
+  </si>
+  <si>
+    <t>(1, 0, Inf)</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>Net Profit</t>
+  </si>
+  <si>
+    <t>Inf</t>
+  </si>
+  <si>
+    <t>Units Upper</t>
+  </si>
+  <si>
+    <t>Determine Upper Limit</t>
+  </si>
+  <si>
+    <t>Upper Bound</t>
+  </si>
+  <si>
+    <t>Lower Bound</t>
+  </si>
+  <si>
+    <t>Arc</t>
+  </si>
+  <si>
+    <t>upper 310,000</t>
+  </si>
+  <si>
+    <t>(c, 0, 0)</t>
+  </si>
+  <si>
+    <t>upper 930,000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="8">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0_);_([$$-409]* \(#,##0\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="&quot;(&quot;0&quot;)&quot;"/>
     <numFmt numFmtId="167" formatCode="&quot;(&quot;0&quot;,0,∞)&quot;"/>
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1363,8 +1539,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1431,8 +1646,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="42">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1927,12 +2158,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39991454817346722"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39991454817346722"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39991454817346722"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39991454817346722"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39991454817346722"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="13" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2298,10 +2659,77 @@
     <xf numFmtId="0" fontId="18" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="41" fontId="36" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="36" fillId="3" borderId="44" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="34" fillId="12" borderId="42" xfId="3" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="35" fillId="13" borderId="43" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="45" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="50" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="36" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="12" borderId="42" xfId="3"/>
+    <xf numFmtId="41" fontId="34" fillId="12" borderId="42" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="4" builtinId="21"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7194,6 +7622,968 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>174638</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>59929</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1AF31B8-E53C-4296-8DCC-9DF99905B89C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1343025" y="1247775"/>
+          <a:ext cx="1365263" cy="1288654"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Grade</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> A</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1300">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>155588</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>88504</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A34ED98-61D9-49E3-BA22-9899730B7BBC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1323975" y="2228850"/>
+          <a:ext cx="1270013" cy="1288654"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Grade</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> B</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1300">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>212738</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>145654</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Oval 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{841A28D7-36A3-4E82-AE9D-E0E736E6576D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4429125" y="381000"/>
+          <a:ext cx="1365263" cy="1288654"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Raisin</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>222263</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>2779</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Oval 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06395674-38FF-48EB-865F-3C8D4F51B168}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4438650" y="2143125"/>
+          <a:ext cx="1365263" cy="1288654"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Juice</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>222263</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>12304</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Oval 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE664123-3725-4625-9F25-BDDE922AAAB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4412876" y="4438650"/>
+          <a:ext cx="1356299" cy="1288654"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Jelly</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>356907</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>93569</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>508574</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>48723</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Oval 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8199A62D-1304-4DA9-B651-BBFA4831055D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7719172" y="2570069"/>
+          <a:ext cx="1361902" cy="1288654"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Dummy Balance Node</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> (Demand)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1300">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>174638</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>72827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177602</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59572513-E018-4D54-99B3-5606C03E9FCA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="6"/>
+          <a:endCxn id="4" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2695962" y="1406327"/>
+          <a:ext cx="1707389" cy="866775"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>174638</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177602</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>120452</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D70401B8-AA6E-4311-A97A-E410D8ADA509}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="6"/>
+          <a:endCxn id="5" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2695962" y="2273102"/>
+          <a:ext cx="1716914" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>174638</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177602</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>129977</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCD559B9-0B56-47D8-9A89-049FF50BFB96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="6"/>
+          <a:endCxn id="6" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2695962" y="2273102"/>
+          <a:ext cx="1716914" cy="2809875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>155588</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>72827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>15677</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48FC6F73-D343-4EDD-8AAF-613FBE99092D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="6"/>
+          <a:endCxn id="4" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2676912" y="1406327"/>
+          <a:ext cx="1726439" cy="2800350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>155588</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>120452</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>15677</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="Straight Arrow Connector 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C779B918-3FF9-487B-8993-9AFEACA19D54}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="6"/>
+          <a:endCxn id="5" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2676912" y="3168452"/>
+          <a:ext cx="1735964" cy="1038225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>155588</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>15677</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>129977</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD9AA0E7-5F48-43E2-9632-246BB93704F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="6"/>
+          <a:endCxn id="6" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676912" y="4206677"/>
+          <a:ext cx="1735964" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>212738</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>72827</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>356907</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>166396</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7C0988D-01A5-41C3-BCE7-E268D217E0A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="6"/>
+          <a:endCxn id="7" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5759650" y="1406327"/>
+          <a:ext cx="1959522" cy="1808069"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>222263</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>120452</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>356907</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>166396</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{563A8B45-9BB9-4E93-B4EF-46666C84C87F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="6"/>
+          <a:endCxn id="7" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5769175" y="3168452"/>
+          <a:ext cx="1949997" cy="45944"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>222263</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>166396</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>356907</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>129977</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Arrow Connector 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E4AF514-4288-4B54-8FCD-28A6AC85459A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="6"/>
+          <a:endCxn id="7" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5769175" y="3214396"/>
+          <a:ext cx="1949997" cy="1868581"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>33</xdr:col>
       <xdr:colOff>420947</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -10187,13 +11577,517 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFBDFB5-E849-45FA-89DB-4B62F157871F}">
+  <dimension ref="B1:Q50"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" style="156" customWidth="1"/>
+    <col min="10" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="L1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M1" s="186">
+        <v>9</v>
+      </c>
+      <c r="N1" s="186">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="149" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="149" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="149" t="s">
+        <v>198</v>
+      </c>
+      <c r="H2" s="149" t="s">
+        <v>194</v>
+      </c>
+      <c r="I2" s="149" t="s">
+        <v>200</v>
+      </c>
+      <c r="J2" s="155" t="s">
+        <v>205</v>
+      </c>
+      <c r="M2" s="155" t="s">
+        <v>197</v>
+      </c>
+      <c r="N2" s="155" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="150">
+        <v>930000</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3" s="151">
+        <v>0.15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>201</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>201</v>
+      </c>
+      <c r="M3" s="187">
+        <v>500000</v>
+      </c>
+      <c r="N3" s="187">
+        <v>400000</v>
+      </c>
+      <c r="P3" s="188">
+        <f>M3 / SUM($M3:$N3) * M$1</f>
+        <v>5</v>
+      </c>
+      <c r="Q3" s="188"/>
+    </row>
+    <row r="4" spans="2:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="150">
+        <v>5270000</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" s="153">
+        <v>0.85</v>
+      </c>
+      <c r="H4" t="s">
+        <v>191</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="L4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M4" s="187">
+        <v>3000000</v>
+      </c>
+      <c r="N4" s="187">
+        <v>1000000</v>
+      </c>
+      <c r="P4" s="188">
+        <f t="shared" ref="P4" si="0">M4 / SUM($M4:$N4) * M$1</f>
+        <v>6.75</v>
+      </c>
+      <c r="Q4" s="188"/>
+    </row>
+    <row r="5" spans="2:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="148" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="152">
+        <f>SUM(C3:C4)</f>
+        <v>6200000</v>
+      </c>
+      <c r="D5" s="148"/>
+      <c r="E5" s="154">
+        <v>1</v>
+      </c>
+      <c r="H5" s="156" t="s">
+        <v>192</v>
+      </c>
+      <c r="I5" s="156">
+        <v>0</v>
+      </c>
+      <c r="L5" s="156" t="s">
+        <v>192</v>
+      </c>
+      <c r="M5" s="187"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="184"/>
+      <c r="P5" s="188"/>
+      <c r="Q5" s="188"/>
+    </row>
+    <row r="6" spans="2:17" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="148"/>
+      <c r="I6" s="148"/>
+    </row>
+    <row r="7" spans="2:17" outlineLevel="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="162" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="160"/>
+      <c r="D9" s="160"/>
+      <c r="E9" s="160"/>
+      <c r="F9" s="160"/>
+      <c r="G9" s="160"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="157" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="159">
+        <v>1240000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="157" t="s">
+        <v>224</v>
+      </c>
+      <c r="C12" s="166">
+        <f>-C3</f>
+        <v>-930000</v>
+      </c>
+      <c r="D12" s="151">
+        <f>-C12 / $C$11</f>
+        <v>0.75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="157" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" s="167">
+        <f>C11 + C12</f>
+        <v>310000</v>
+      </c>
+      <c r="D13" s="151">
+        <f>C13 / $C$11</f>
+        <v>0.25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="157"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15" s="157" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" s="167">
+        <f>C4</f>
+        <v>5270000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="157" t="s">
+        <v>204</v>
+      </c>
+      <c r="C16" s="168">
+        <f>C13 / C15</f>
+        <v>5.8823529411764705E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="157"/>
+      <c r="F17" s="157"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="176" t="s">
+        <v>219</v>
+      </c>
+      <c r="F18" s="157"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="157" t="str">
+        <f>"*There must be " &amp; TEXT(C16, "0.00%") &amp; " (Total of "&amp; TEXT(C13, "#,###")&amp; ") of grade B's total supply that are on tier 8, which raisins are able to use since it satisfies the minimum points."</f>
+        <v>*There must be 5.88% (Total of 310,000) of grade B's total supply that are on tier 8, which raisins are able to use since it satisfies the minimum points.</v>
+      </c>
+      <c r="F19" s="157"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="157" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="157" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="157" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="157"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="162" t="s">
+        <v>221</v>
+      </c>
+      <c r="C24" s="160"/>
+      <c r="D24" s="160"/>
+      <c r="E24" s="160"/>
+    </row>
+    <row r="26" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="155" t="s">
+        <v>208</v>
+      </c>
+      <c r="C26" s="155" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="172" t="s">
+        <v>197</v>
+      </c>
+      <c r="C27" s="173">
+        <v>0.45</v>
+      </c>
+      <c r="D27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="174" t="s">
+        <v>196</v>
+      </c>
+      <c r="C28" s="175">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="155"/>
+      <c r="C30" s="155" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="155" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" s="155" t="s">
+        <v>192</v>
+      </c>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30" s="156"/>
+      <c r="K30" s="156"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="169" t="s">
+        <v>193</v>
+      </c>
+      <c r="C31" s="170">
+        <v>6.5</v>
+      </c>
+      <c r="D31" s="170">
+        <v>14</v>
+      </c>
+      <c r="E31" s="171">
+        <v>18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>215</v>
+      </c>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31" s="156"/>
+      <c r="K31" s="156"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32" s="156"/>
+      <c r="K32" s="156"/>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B33" s="163" t="s">
+        <v>207</v>
+      </c>
+      <c r="C33" s="163"/>
+      <c r="D33" s="163"/>
+      <c r="E33" s="163"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33" s="156"/>
+      <c r="K33" s="156"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>197</v>
+      </c>
+      <c r="C34" s="158">
+        <f>1 - C35</f>
+        <v>0.75</v>
+      </c>
+      <c r="D34" s="158">
+        <f t="shared" ref="D34:E34" si="1">1 - D35</f>
+        <v>0.24999999999999978</v>
+      </c>
+      <c r="E34" s="158">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>214</v>
+      </c>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34" s="156"/>
+      <c r="K34" s="156"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>196</v>
+      </c>
+      <c r="C35" s="158">
+        <f>D13</f>
+        <v>0.25</v>
+      </c>
+      <c r="D35" s="158">
+        <v>0.75000000000000022</v>
+      </c>
+      <c r="E35" s="158">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>217</v>
+      </c>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35" s="156"/>
+      <c r="K35" s="156"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>206</v>
+      </c>
+      <c r="C36" s="161">
+        <f>(C35 * $C$28) + (C34 * $C$27)</f>
+        <v>0.4</v>
+      </c>
+      <c r="D36" s="161">
+        <f t="shared" ref="D36:E36" si="2">(D35 * $C$28) + (D34 * $C$27)</f>
+        <v>0.29999999999999993</v>
+      </c>
+      <c r="E36" s="161">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36" s="156"/>
+      <c r="K36" s="156"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="103" t="s">
+        <v>210</v>
+      </c>
+      <c r="C37" s="164">
+        <f>C31 * $C$36</f>
+        <v>2.6</v>
+      </c>
+      <c r="D37" s="164">
+        <f>D36 * D31</f>
+        <v>4.1999999999999993</v>
+      </c>
+      <c r="E37" s="164">
+        <f>E36 * E31</f>
+        <v>4.5</v>
+      </c>
+      <c r="F37" s="165" t="s">
+        <v>218</v>
+      </c>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37" s="156"/>
+      <c r="K37" s="156"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38" s="156"/>
+      <c r="K38" s="156"/>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44" s="156"/>
+      <c r="K44" s="156"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45" s="156"/>
+      <c r="K45" s="156"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46" s="156"/>
+      <c r="K46" s="156"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47" s="156"/>
+      <c r="K47" s="156"/>
+    </row>
+    <row r="48" spans="2:11" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48" s="156"/>
+      <c r="K48" s="156"/>
+    </row>
+    <row r="49" spans="8:11" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49" s="156"/>
+      <c r="K49" s="156"/>
+    </row>
+    <row r="50" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50" s="156"/>
+      <c r="K50" s="156"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F6EB8B-EEA2-48C7-A135-DB48C73C0E00}">
   <dimension ref="B2:AK34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -11176,15 +13070,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC69D54E-00BB-4469-9873-ACE66827EA4B}">
   <dimension ref="A1:BJ52"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D34" sqref="A34:D35"/>
-    </sheetView>
-    <sheetView showGridLines="0" zoomScale="81" zoomScaleNormal="81" workbookViewId="1">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -12955,12 +14846,281 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA39DA1-A367-4818-9935-35E5EE7A4AC9}">
+  <dimension ref="A2:P36"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B41:B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C2" s="178" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" s="178"/>
+      <c r="J2" s="178" t="s">
+        <v>227</v>
+      </c>
+      <c r="K2" s="178"/>
+    </row>
+    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+    </row>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C4" s="179"/>
+      <c r="D4" s="179"/>
+      <c r="J4" s="179"/>
+      <c r="K4" s="179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D8" s="150">
+        <v>930000</v>
+      </c>
+      <c r="H8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>237</v>
+      </c>
+      <c r="N12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="P13" s="150">
+        <f>-SUM(D8,D27)</f>
+        <v>-6200000</v>
+      </c>
+    </row>
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="I15" s="185" t="str">
+        <f>$K$35</f>
+        <v>(-0.14, 0.00, 2,660,000.00)</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="I16" s="185"/>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I17" s="185"/>
+      <c r="M17" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I18" s="185"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I19" s="185" t="str">
+        <f>$K$35</f>
+        <v>(-0.14, 0.00, 2,660,000.00)</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>238</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="D27" s="150">
+        <v>5270000</v>
+      </c>
+      <c r="I27" s="184" t="str">
+        <f>$K$36</f>
+        <v>(0.43, 0.00, 3,780,000.00)</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="177" t="s">
+        <v>233</v>
+      </c>
+      <c r="C32" s="177"/>
+      <c r="H32" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="182" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" s="182" t="s">
+        <v>232</v>
+      </c>
+      <c r="D33" s="149"/>
+      <c r="E33" s="149" t="s">
+        <v>229</v>
+      </c>
+      <c r="F33" s="149"/>
+      <c r="G33" s="149"/>
+      <c r="H33" s="149" t="s">
+        <v>230</v>
+      </c>
+      <c r="I33" s="183" t="s">
+        <v>235</v>
+      </c>
+      <c r="J33" s="183" t="s">
+        <v>234</v>
+      </c>
+      <c r="K33" s="155" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>190</v>
+      </c>
+      <c r="B34" s="181">
+        <v>6.5</v>
+      </c>
+      <c r="C34" s="150" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" t="s">
+        <v>190</v>
+      </c>
+      <c r="E34" s="147">
+        <v>1.4</v>
+      </c>
+      <c r="F34" s="147"/>
+      <c r="G34" s="147"/>
+      <c r="H34" s="147">
+        <v>0.35</v>
+      </c>
+      <c r="I34" s="180">
+        <v>0</v>
+      </c>
+      <c r="J34" s="150" t="str">
+        <f>C34</f>
+        <v>Inf</v>
+      </c>
+      <c r="K34" t="str" cm="1">
+        <f t="array" ref="K34">"(" &amp; _xlfn.TEXTJOIN(", ", FALSE, TEXT(H34:J34, "#,##0.00")) &amp; ")"</f>
+        <v>(0.35, 0.00, Inf)</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>191</v>
+      </c>
+      <c r="B35" s="181">
+        <v>14</v>
+      </c>
+      <c r="C35" s="150">
+        <v>190000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>191</v>
+      </c>
+      <c r="E35" s="147">
+        <v>2.46</v>
+      </c>
+      <c r="F35" s="147"/>
+      <c r="G35" s="147"/>
+      <c r="H35" s="147">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="I35" s="180">
+        <v>0</v>
+      </c>
+      <c r="J35" s="150">
+        <f>B35 * C35</f>
+        <v>2660000</v>
+      </c>
+      <c r="K35" t="str" cm="1">
+        <f t="array" ref="K35">"(" &amp; _xlfn.TEXTJOIN(", ", FALSE, TEXT(H35:J35, "#,##0.00")) &amp; ")"</f>
+        <v>(-0.14, 0.00, 2,660,000.00)</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>192</v>
+      </c>
+      <c r="B36" s="181">
+        <v>18</v>
+      </c>
+      <c r="C36" s="150">
+        <v>210000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>192</v>
+      </c>
+      <c r="E36" s="147">
+        <v>2.35</v>
+      </c>
+      <c r="F36" s="147"/>
+      <c r="G36" s="147"/>
+      <c r="H36" s="147">
+        <v>0.43</v>
+      </c>
+      <c r="I36" s="180">
+        <v>0</v>
+      </c>
+      <c r="J36" s="150">
+        <f>B36 * C36</f>
+        <v>3780000</v>
+      </c>
+      <c r="K36" t="str" cm="1">
+        <f t="array" ref="K36">"(" &amp; _xlfn.TEXTJOIN(", ", FALSE, TEXT(H36:J36, "#,##0.00")) &amp; ")"</f>
+        <v>(0.43, 0.00, 3,780,000.00)</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1DB666-5CF3-4627-8B70-A129646F75C2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599F1D43-9BD8-4A09-A61C-254B47A47DFE}">
   <dimension ref="B1:K22"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13347,12 +15507,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70FBFC5-285A-4C09-B287-071ADBFF8F1F}">
   <dimension ref="B1:M22"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13741,12 +15900,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63517073-B66B-40C8-B48B-0323E1700D94}">
   <dimension ref="A1:AI50"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="81" zoomScaleNormal="81" workbookViewId="0"/>
-    <sheetView showGridLines="0" zoomScale="77" zoomScaleNormal="77" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Reworking (code/rmd) Problem 1
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 02/Network Flow Graphs.xlsx
+++ b/03 - Homework/HW 02/Network Flow Graphs.xlsx
@@ -5,23 +5,75 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.carpenter\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.carpenter\OneDrive - the Chickasaw Nation\Documents\GitHub\OU-DSA\Metaheuristics\03 - Homework\HW 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80FFF920-F72B-4BFB-A688-D0590BC528E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662D3C07-FF0C-45F8-BF75-07F7834DABAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem 1(b) Scratch" sheetId="6" r:id="rId1"/>
-    <sheet name="Problem 3" sheetId="4" r:id="rId2"/>
-    <sheet name="Problem 4" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="8" r:id="rId5"/>
-    <sheet name="P4 Scratch" sheetId="3" state="hidden" r:id="rId6"/>
-    <sheet name="P3 Scratch" sheetId="5" state="hidden" r:id="rId7"/>
-    <sheet name="P4 V1" sheetId="1" state="hidden" r:id="rId8"/>
+    <sheet name="Problem 1 LP" sheetId="9" r:id="rId2"/>
+    <sheet name="Problem 3" sheetId="4" r:id="rId3"/>
+    <sheet name="Problem 4" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId6"/>
+    <sheet name="P4 Scratch" sheetId="3" state="hidden" r:id="rId7"/>
+    <sheet name="P3 Scratch" sheetId="5" state="hidden" r:id="rId8"/>
+    <sheet name="P4 V1" sheetId="1" state="hidden" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="OpenSolver_ChosenSolver" localSheetId="1" hidden="1">CBC</definedName>
+    <definedName name="OpenSolver_DualsNewSheet" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="OpenSolver_LinearityCheck" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Problem 1 LP'!$L$6:$M$8</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Problem 1 LP'!$L$6:$L$7</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Problem 1 LP'!$M$7</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Problem 1 LP'!$M$8</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Problem 1 LP'!$N$6:$N$8</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Problem 1 LP'!$Y$11:$Y$14</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Problem 1 LP'!$Y$6:$Y$8</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">6</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Problem 1 LP'!$AA$3</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Problem 1 LP'!$R$6:$R$8</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Problem 1 LP'!$AA$11:$AA$14</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Problem 1 LP'!$AA$6:$AA$8</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -63,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="256">
   <si>
     <t>Labor Sources</t>
   </si>
@@ -1281,12 +1333,60 @@
   <si>
     <t>upper 930,000</t>
   </si>
+  <si>
+    <t>Total per Grade</t>
+  </si>
+  <si>
+    <t>Grade A Points</t>
+  </si>
+  <si>
+    <t>Grade B Points</t>
+  </si>
+  <si>
+    <t>Total Weighted Points</t>
+  </si>
+  <si>
+    <t>==</t>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>Net Profit / Unit</t>
+  </si>
+  <si>
+    <t>Contribution / Unit</t>
+  </si>
+  <si>
+    <t>Total Profit</t>
+  </si>
+  <si>
+    <t>Pounds/Product</t>
+  </si>
+  <si>
+    <t>Product Limit</t>
+  </si>
+  <si>
+    <t>Upper Limit</t>
+  </si>
+  <si>
+    <t>Grade A Total</t>
+  </si>
+  <si>
+    <t>Grade B Total</t>
+  </si>
+  <si>
+    <t>Jelly Grade A 0</t>
+  </si>
+  <si>
+    <t>Total Grade Lim</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
@@ -1295,6 +1395,7 @@
     <numFmt numFmtId="167" formatCode="&quot;(&quot;0&quot;,0,∞)&quot;"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="0.E+00"/>
   </numFmts>
   <fonts count="39" x14ac:knownFonts="1">
     <font>
@@ -1579,7 +1680,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1662,8 +1763,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="51">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -2285,6 +2398,93 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2293,7 +2493,7 @@
     <xf numFmtId="0" fontId="34" fillId="12" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="13" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="189">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2723,6 +2923,50 @@
     <xf numFmtId="0" fontId="34" fillId="12" borderId="42" xfId="3"/>
     <xf numFmtId="41" fontId="34" fillId="12" borderId="42" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="35" fillId="15" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="35" fillId="15" borderId="51" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="41" fontId="36" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="34" fillId="11" borderId="53" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="34" fillId="11" borderId="42" xfId="3" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="34" fillId="11" borderId="52" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="34" fillId="11" borderId="54" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="34" fillId="11" borderId="55" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="34" fillId="11" borderId="56" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="28" fillId="4" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="28" fillId="4" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="28" fillId="4" borderId="39" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="4" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="4" borderId="57" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="0" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="35" fillId="13" borderId="43" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="36" fillId="3" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2745,6 +2989,1474 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="90" name="OpenSolver1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{204390B4-F56D-4DB0-B2D3-A76AC4A8B0B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5819775" y="1333500"/>
+          <a:ext cx="1695450" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF00FF">
+            <a:alpha val="40000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF00FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="91" name="OpenSolver2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43E889B1-D082-419A-8C33-C26CE8361F4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15325725" y="381000"/>
+          <a:ext cx="981075" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF00FF"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF00FF"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>239710</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="OpenSolver3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F355AF3C-874B-4296-A0D5-9D3FC26F01C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15316200" y="304800"/>
+          <a:ext cx="249235" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:alpha val="80000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="12700" tIns="0" rIns="12700" bIns="0" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>max </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="93" name="OpenSolverL6:L7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAFC943A-76D4-4CF6-9FDB-021D62F3ACCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5819775" y="1333500"/>
+          <a:ext cx="847725" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="0000FF"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1≤</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="94" name="OpenSolverM7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CE71728-F7B0-47C6-8EAB-29FEFA17BC05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6667500" y="1524000"/>
+          <a:ext cx="847725" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="008000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="008000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1≤</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="95" name="OpenSolverM8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4235D59F-5432-4DC2-A534-109D9CF88FA3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6667500" y="1714500"/>
+          <a:ext cx="847725" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="9900CC"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="9900CC"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1≤</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="96" name="OpenSolver7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63A1AE25-58EC-4765-8E49-E6C3CA4DA89F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7515225" y="1333500"/>
+          <a:ext cx="847725" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="800000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="800000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="97" name="OpenSolver8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A26DAEB9-95AB-41B1-9FFB-BBC216533784}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8658225" y="1333500"/>
+          <a:ext cx="781050" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="800000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="800000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>≤</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="98" name="OpenSolver9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2C3FCC0-4CEA-4D1E-818D-9DF52EF735F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="96" idx="3"/>
+          <a:endCxn id="97" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8362950" y="1619250"/>
+          <a:ext cx="295275" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="800000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>804863</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>42863</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="99" name="OpenSolver10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77F40F5D-8232-4760-A4BD-005EB81A95E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8320088" y="1492250"/>
+          <a:ext cx="381000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="100" name="OpenSolver11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{973590FB-51F2-44FC-AE9B-4529A6A8D7FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14182725" y="2286000"/>
+          <a:ext cx="847725" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="00CC33"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="00CC33"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="OpenSolver12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD19B822-F191-4779-A251-C3E2629F3FFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15325725" y="2286000"/>
+          <a:ext cx="981075" cy="762000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="00CC33"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="00CC33"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>=</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="102" name="OpenSolver13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE4568E2-E527-467D-A91C-8E5458A738FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="100" idx="3"/>
+          <a:endCxn id="101" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15030450" y="2667000"/>
+          <a:ext cx="295275" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="00CC33"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>804863</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>42863</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="103" name="OpenSolver14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DB9A4E7-58D3-4647-A9A8-34FEA2A7E96E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14987588" y="2540000"/>
+          <a:ext cx="381000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="104" name="OpenSolver15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8749C426-8914-4505-A2FB-B2BCDCAF2C60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14182725" y="1333500"/>
+          <a:ext cx="847725" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF6600"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FF6600"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="105" name="OpenSolver16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE92B641-2C6F-446D-B4FF-B2D4628B79E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15325725" y="1333500"/>
+          <a:ext cx="981075" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="FF6600"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="25400" tIns="25400" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF6600"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>≥</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="106" name="OpenSolver17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC8ACD58-DE02-4EF1-A5F9-39D7C8253667}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="104" idx="3"/>
+          <a:endCxn id="105" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15030450" y="1619250"/>
+          <a:ext cx="295275" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:srgbClr val="FF6600"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>804863</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>42863</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="107" name="OpenSolver18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A56F3D2-A3FE-4E71-A2E3-4759D2A9FFD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14987588" y="1492250"/>
+          <a:ext cx="381000" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="12700" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:miter lim="800000"/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5283,7 +6995,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7618,7 +9330,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -8580,7 +10292,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -11580,8 +13292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFBDFB5-E849-45FA-89DB-4B62F157871F}">
   <dimension ref="B1:Q50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -12082,6 +13794,453 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E3DAB5-08C1-466A-BE0C-2503F8287B81}">
+  <dimension ref="A2:AA14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="8" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="6" width="2.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="8" width="12.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="2.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="4.42578125" style="185" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.7109375" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" style="96" customWidth="1"/>
+    <col min="24" max="25" width="12.7109375" customWidth="1"/>
+    <col min="26" max="26" width="4.42578125" style="185" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" customWidth="1"/>
+    <col min="30" max="31" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L2" s="185" t="str">
+        <f t="shared" ref="L2:M2" si="0">L5</f>
+        <v>Grade A</v>
+      </c>
+      <c r="M2" s="185" t="str">
+        <f t="shared" si="0"/>
+        <v>Grade B</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="C3" s="147"/>
+      <c r="D3" s="147"/>
+      <c r="G3" s="156"/>
+      <c r="H3" s="156"/>
+      <c r="K3" t="s">
+        <v>199</v>
+      </c>
+      <c r="L3" s="186">
+        <v>9</v>
+      </c>
+      <c r="M3" s="186">
+        <v>5</v>
+      </c>
+      <c r="O3" s="184"/>
+      <c r="Z3" s="184" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA3" s="219">
+        <f>U9</f>
+        <v>1424865.0619485416</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" ht="45" x14ac:dyDescent="0.25">
+      <c r="B5" s="149" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="149" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="149" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" s="149" t="s">
+        <v>194</v>
+      </c>
+      <c r="H5" s="149" t="s">
+        <v>200</v>
+      </c>
+      <c r="K5" s="149" t="s">
+        <v>194</v>
+      </c>
+      <c r="L5" s="149" t="s">
+        <v>197</v>
+      </c>
+      <c r="M5" s="149" t="s">
+        <v>196</v>
+      </c>
+      <c r="N5" s="215" t="s">
+        <v>174</v>
+      </c>
+      <c r="O5" s="215"/>
+      <c r="P5" s="215" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q5" s="215" t="s">
+        <v>250</v>
+      </c>
+      <c r="R5" s="215" t="s">
+        <v>251</v>
+      </c>
+      <c r="S5" s="149" t="s">
+        <v>247</v>
+      </c>
+      <c r="T5" s="149" t="s">
+        <v>246</v>
+      </c>
+      <c r="U5" s="149" t="s">
+        <v>248</v>
+      </c>
+      <c r="W5" s="155" t="s">
+        <v>241</v>
+      </c>
+      <c r="X5" s="155" t="s">
+        <v>242</v>
+      </c>
+      <c r="Y5" s="215" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z5" s="215"/>
+      <c r="AA5" s="215" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" s="150">
+        <v>930000</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>201</v>
+      </c>
+      <c r="L6" s="196">
+        <v>399665.97246145637</v>
+      </c>
+      <c r="M6" s="199">
+        <v>0</v>
+      </c>
+      <c r="N6" s="212">
+        <f>SUM(L6:M6)</f>
+        <v>399665.97246145637</v>
+      </c>
+      <c r="O6" s="209" t="s">
+        <v>161</v>
+      </c>
+      <c r="P6" s="202">
+        <v>6.5</v>
+      </c>
+      <c r="Q6" s="203">
+        <v>9.9999999999999996E+27</v>
+      </c>
+      <c r="R6" s="204">
+        <f>Q6 * P6</f>
+        <v>6.5000000000000001E+28</v>
+      </c>
+      <c r="S6" s="181">
+        <v>1.4</v>
+      </c>
+      <c r="T6" s="181">
+        <v>0.35</v>
+      </c>
+      <c r="U6" s="150">
+        <f>T6 * N6</f>
+        <v>139883.09036150973</v>
+      </c>
+      <c r="W6" s="193">
+        <f>IFERROR(L6 / SUM($L6:$M6) * L$3, 1)</f>
+        <v>9</v>
+      </c>
+      <c r="X6" s="193">
+        <f t="shared" ref="X6:X8" si="1">IFERROR(M6 / SUM($L6:$M6) * M$3, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="216">
+        <f>SUM(W6:X6)</f>
+        <v>9</v>
+      </c>
+      <c r="Z6" s="216" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA6" s="216">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="150">
+        <v>5270000</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>191</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>191</v>
+      </c>
+      <c r="L7" s="197">
+        <v>530334.02753854357</v>
+      </c>
+      <c r="M7" s="200">
+        <v>1591002.2185220558</v>
+      </c>
+      <c r="N7" s="213">
+        <f t="shared" ref="N7:N8" si="2">SUM(L7:M7)</f>
+        <v>2121336.2460605996</v>
+      </c>
+      <c r="O7" s="210" t="s">
+        <v>161</v>
+      </c>
+      <c r="P7" s="205">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="205">
+        <v>190000</v>
+      </c>
+      <c r="R7" s="206">
+        <f>Q7 * P7</f>
+        <v>2660000</v>
+      </c>
+      <c r="S7" s="181">
+        <v>2.46</v>
+      </c>
+      <c r="T7" s="181">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="U7" s="150">
+        <f t="shared" ref="U7:U8" si="3">T7 * N7</f>
+        <v>-296987.074448484</v>
+      </c>
+      <c r="W7" s="193">
+        <f t="shared" ref="W7:W8" si="4">IFERROR(L7 / SUM($L7:$M7) * L$3, 1)</f>
+        <v>2.2499998558505481</v>
+      </c>
+      <c r="X7" s="193">
+        <f t="shared" si="1"/>
+        <v>3.7500000800830282</v>
+      </c>
+      <c r="Y7" s="217">
+        <f t="shared" ref="Y7:Y8" si="5">SUM(W7:X7)</f>
+        <v>5.9999999359335767</v>
+      </c>
+      <c r="Z7" s="217" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA7" s="217">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="B8" s="148" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="152">
+        <f>SUM(C6:C7)</f>
+        <v>6200000</v>
+      </c>
+      <c r="D8" s="148"/>
+      <c r="G8" s="156" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" s="156">
+        <v>0</v>
+      </c>
+      <c r="K8" s="156" t="s">
+        <v>192</v>
+      </c>
+      <c r="L8" s="198">
+        <v>0</v>
+      </c>
+      <c r="M8" s="201">
+        <v>3678997.781477944</v>
+      </c>
+      <c r="N8" s="214">
+        <f t="shared" si="2"/>
+        <v>3678997.781477944</v>
+      </c>
+      <c r="O8" s="211" t="s">
+        <v>161</v>
+      </c>
+      <c r="P8" s="207">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="207">
+        <v>210000</v>
+      </c>
+      <c r="R8" s="208">
+        <f>Q8 * P8</f>
+        <v>3780000</v>
+      </c>
+      <c r="S8" s="181">
+        <v>2.35</v>
+      </c>
+      <c r="T8" s="181">
+        <v>0.43</v>
+      </c>
+      <c r="U8" s="150">
+        <f t="shared" si="3"/>
+        <v>1581969.0460355158</v>
+      </c>
+      <c r="W8" s="193">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="X8" s="193">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="Y8" s="218">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="Z8" s="218" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA8" s="218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="K9" s="148" t="s">
+        <v>240</v>
+      </c>
+      <c r="L9" s="152">
+        <f>SUM(L6:L8)</f>
+        <v>930000</v>
+      </c>
+      <c r="M9" s="152">
+        <f>SUM(M6:M8)</f>
+        <v>5270000</v>
+      </c>
+      <c r="N9" s="192">
+        <f>SUM(N6:N8)</f>
+        <v>6200000</v>
+      </c>
+      <c r="O9" s="191"/>
+      <c r="P9" s="192"/>
+      <c r="Q9" s="192"/>
+      <c r="R9" s="192"/>
+      <c r="S9" s="148"/>
+      <c r="T9" s="148"/>
+      <c r="U9" s="220">
+        <f>SUM(U6:U8)</f>
+        <v>1424865.0619485416</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="G10" s="156"/>
+      <c r="H10" s="156"/>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="K11" s="189" t="s">
+        <v>174</v>
+      </c>
+      <c r="L11" s="190">
+        <f>SUM(L9:M9)</f>
+        <v>6200000</v>
+      </c>
+      <c r="M11" s="150"/>
+      <c r="O11" s="194"/>
+      <c r="X11" s="184" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y11" s="150">
+        <f>L11</f>
+        <v>6200000</v>
+      </c>
+      <c r="Z11" s="194" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA11" s="150">
+        <f>C8</f>
+        <v>6200000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="X12" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y12" s="180">
+        <f>L8</f>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="195" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="O13" s="195"/>
+      <c r="X13" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y13" s="150">
+        <f>L9</f>
+        <v>930000</v>
+      </c>
+      <c r="Z13" s="195" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA13" s="150">
+        <f>C6</f>
+        <v>930000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="X14" t="s">
+        <v>253</v>
+      </c>
+      <c r="Y14" s="150">
+        <f>M9</f>
+        <v>5270000</v>
+      </c>
+      <c r="Z14" s="195" t="s">
+        <v>244</v>
+      </c>
+      <c r="AA14" s="150">
+        <f>C7</f>
+        <v>5270000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F6EB8B-EEA2-48C7-A135-DB48C73C0E00}">
   <dimension ref="B2:AK34"/>
   <sheetViews>
@@ -13070,7 +15229,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC69D54E-00BB-4469-9873-ACE66827EA4B}">
   <dimension ref="A1:BJ52"/>
   <sheetViews>
@@ -14846,12 +17005,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA39DA1-A367-4818-9935-35E5EE7A4AC9}">
   <dimension ref="A2:P36"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B42" sqref="B41:B42"/>
+      <selection activeCell="H34" activeCellId="1" sqref="E34:E36 H34:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15104,7 +17263,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1DB666-5CF3-4627-8B70-A129646F75C2}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -15116,7 +17275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599F1D43-9BD8-4A09-A61C-254B47A47DFE}">
   <dimension ref="B1:K22"/>
   <sheetViews>
@@ -15507,7 +17666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E70FBFC5-285A-4C09-B287-071ADBFF8F1F}">
   <dimension ref="B1:M22"/>
   <sheetViews>
@@ -15900,7 +18059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63517073-B66B-40C8-B48B-0323E1700D94}">
   <dimension ref="A1:AI50"/>
   <sheetViews>

</xml_diff>

<commit_message>
Constraints formulated less avg points
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 02/Network Flow Graphs.xlsx
+++ b/03 - Homework/HW 02/Network Flow Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.carpenter\OneDrive - the Chickasaw Nation\Documents\GitHub\OU-DSA\Metaheuristics\03 - Homework\HW 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662D3C07-FF0C-45F8-BF75-07F7834DABAA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA83A635-F3AB-457A-81E1-C9EF5AB9B533}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="257">
   <si>
     <t>Labor Sources</t>
   </si>
@@ -1381,6 +1381,9 @@
   <si>
     <t>Total Grade Lim</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
@@ -1395,7 +1398,7 @@
     <numFmt numFmtId="167" formatCode="&quot;(&quot;0&quot;,0,∞)&quot;"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="0.E+00"/>
+    <numFmt numFmtId="170" formatCode="0.E+00"/>
   </numFmts>
   <fonts count="39" x14ac:knownFonts="1">
     <font>
@@ -2941,8 +2944,8 @@
     <xf numFmtId="41" fontId="34" fillId="11" borderId="55" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="34" fillId="11" borderId="56" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -13798,7 +13801,7 @@
   <dimension ref="A2:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -13857,6 +13860,23 @@
         <v>1424865.0619485416</v>
       </c>
     </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="N4" s="185" t="s">
+        <v>256</v>
+      </c>
+      <c r="O4" s="185" t="s">
+        <v>256</v>
+      </c>
+      <c r="P4" s="185" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q4" s="185" t="s">
+        <v>256</v>
+      </c>
+      <c r="R4" s="185" t="s">
+        <v>256</v>
+      </c>
+    </row>
     <row r="5" spans="2:27" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="149" t="s">
         <v>208</v>
@@ -14171,6 +14191,9 @@
       </c>
       <c r="M11" s="150"/>
       <c r="O11" s="194"/>
+      <c r="W11" s="96" t="s">
+        <v>256</v>
+      </c>
       <c r="X11" s="184" t="s">
         <v>255</v>
       </c>
@@ -14187,6 +14210,9 @@
       </c>
     </row>
     <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="W12" s="96" t="s">
+        <v>256</v>
+      </c>
       <c r="X12" t="s">
         <v>254</v>
       </c>
@@ -14203,6 +14229,9 @@
     </row>
     <row r="13" spans="2:27" x14ac:dyDescent="0.25">
       <c r="O13" s="195"/>
+      <c r="W13" s="96" t="s">
+        <v>256</v>
+      </c>
       <c r="X13" t="s">
         <v>252</v>
       </c>
@@ -14219,6 +14248,9 @@
       </c>
     </row>
     <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="W14" s="96" t="s">
+        <v>256</v>
+      </c>
       <c r="X14" t="s">
         <v>253</v>
       </c>

</xml_diff>

<commit_message>
Per Product Basis (Working)
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 02/Network Flow Graphs.xlsx
+++ b/03 - Homework/HW 02/Network Flow Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.carpenter\OneDrive - the Chickasaw Nation\Documents\GitHub\OU-DSA\Metaheuristics\03 - Homework\HW 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5675E32-4D80-4483-A718-A12AE28DB964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87281062-8351-4C42-BC8F-6C3BF0EA7D6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="256">
   <si>
     <t>Labor Sources</t>
   </si>
@@ -1337,12 +1337,6 @@
     <t>Total per Grade</t>
   </si>
   <si>
-    <t>Total Profit</t>
-  </si>
-  <si>
-    <t>Pounds/Product</t>
-  </si>
-  <si>
     <t xml:space="preserve">&gt;= </t>
   </si>
   <si>
@@ -1365,9 +1359,6 @@
   </si>
   <si>
     <t>Weighted Avg Limit</t>
-  </si>
-  <si>
-    <t>Net Profit / Pound</t>
   </si>
   <si>
     <t>Total Lbs</t>
@@ -1535,7 +1526,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="9">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
@@ -1544,8 +1535,7 @@
     <numFmt numFmtId="167" formatCode="&quot;(&quot;0&quot;,0,∞)&quot;"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="183" formatCode="_(* #,##0.000000000000000_);_(* \(#,##0.000000000000000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="198" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="173" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="42" x14ac:knownFonts="1">
     <font>
@@ -1945,7 +1935,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -2569,67 +2559,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color theme="0" tint="-4.9989318521683403E-2"/>
       </left>
       <right style="thin">
@@ -2656,6 +2585,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14990691854609822"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14993743705557422"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2664,7 +2619,7 @@
     <xf numFmtId="0" fontId="34" fillId="12" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="13" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="221">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3095,12 +3050,7 @@
     <xf numFmtId="41" fontId="34" fillId="12" borderId="42" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="36" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="41" fontId="34" fillId="11" borderId="52" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="34" fillId="11" borderId="42" xfId="3" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="34" fillId="11" borderId="51" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="34" fillId="11" borderId="53" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="34" fillId="11" borderId="54" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="34" fillId="11" borderId="55" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="35" fillId="13" borderId="43" xfId="4" applyNumberFormat="1"/>
@@ -3113,11 +3063,9 @@
     <xf numFmtId="0" fontId="28" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="56" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="198" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="51" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="36" fillId="3" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3126,11 +3074,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="39" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" wrapText="1"/>
     </xf>
@@ -3144,6 +3088,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="53" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="9" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -12504,10 +12458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E3DAB5-08C1-466A-BE0C-2503F8287B81}">
-  <dimension ref="A2:AD11"/>
+  <dimension ref="A2:AE31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11:P11"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -12523,27 +12477,28 @@
     <col min="12" max="13" width="12.7109375" customWidth="1"/>
     <col min="14" max="14" width="2.7109375" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" customWidth="1"/>
     <col min="17" max="17" width="12.7109375" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="185" customWidth="1"/>
-    <col min="19" max="19" width="2.7109375" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="3.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="11.7109375" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" customWidth="1"/>
-    <col min="24" max="24" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.7109375" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" style="96" customWidth="1"/>
-    <col min="27" max="27" width="12.7109375" customWidth="1"/>
-    <col min="28" max="28" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="4.42578125" style="185" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.7109375" customWidth="1"/>
-    <col min="32" max="32" width="4.7109375" customWidth="1"/>
-    <col min="35" max="36" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.7109375" style="185" customWidth="1"/>
+    <col min="21" max="21" width="2.7109375" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="3.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="11.7109375" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" customWidth="1"/>
+    <col min="26" max="26" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.7109375" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="12.7109375" style="96" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.42578125" style="185" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="33" max="33" width="4.7109375" customWidth="1"/>
+    <col min="36" max="37" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="11:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="11:30" x14ac:dyDescent="0.25">
       <c r="L2" s="185" t="str">
         <f t="shared" ref="L2:M2" si="0">L5</f>
         <v>Grade A</v>
@@ -12553,9 +12508,9 @@
         <v>Grade B</v>
       </c>
     </row>
-    <row r="3" spans="11:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="11:30" x14ac:dyDescent="0.25">
       <c r="K3" s="184" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L3" s="186">
         <v>9</v>
@@ -12563,27 +12518,26 @@
       <c r="M3" s="186">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="11:29" x14ac:dyDescent="0.25">
-      <c r="O4" s="163" t="s">
-        <v>254</v>
-      </c>
-      <c r="P4" s="163"/>
-      <c r="Q4" s="163"/>
+      <c r="AB3" s="184"/>
+    </row>
+    <row r="4" spans="11:30" x14ac:dyDescent="0.25">
+      <c r="Q4" s="163" t="s">
+        <v>251</v>
+      </c>
       <c r="R4" s="163"/>
-      <c r="V4" s="216" t="s">
-        <v>255</v>
-      </c>
-      <c r="W4" s="216"/>
-      <c r="X4" s="216"/>
-      <c r="Z4" s="217" t="s">
-        <v>256</v>
-      </c>
-      <c r="AA4" s="218"/>
-      <c r="AB4" s="218"/>
-      <c r="AC4" s="218"/>
-    </row>
-    <row r="5" spans="11:29" ht="30" x14ac:dyDescent="0.25">
+      <c r="S4" s="163"/>
+      <c r="T4" s="163"/>
+      <c r="X4" s="205" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y4" s="205"/>
+      <c r="Z4" s="205"/>
+      <c r="AC4" s="206" t="s">
+        <v>253</v>
+      </c>
+      <c r="AD4" s="207"/>
+    </row>
+    <row r="5" spans="11:30" ht="30" x14ac:dyDescent="0.25">
       <c r="K5" s="149" t="s">
         <v>194</v>
       </c>
@@ -12593,245 +12547,295 @@
       <c r="M5" s="149" t="s">
         <v>196</v>
       </c>
-      <c r="O5" s="208" t="s">
+      <c r="O5" s="149" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q5" s="201" t="s">
+        <v>242</v>
+      </c>
+      <c r="R5" s="202"/>
+      <c r="S5" s="201" t="s">
+        <v>243</v>
+      </c>
+      <c r="T5" s="202" t="s">
+        <v>250</v>
+      </c>
+      <c r="V5" s="155" t="s">
         <v>244</v>
       </c>
-      <c r="P5" s="209"/>
-      <c r="Q5" s="208" t="s">
-        <v>245</v>
-      </c>
-      <c r="R5" s="209" t="s">
-        <v>253</v>
-      </c>
-      <c r="T5" s="155" t="s">
+      <c r="X5" s="196" t="s">
         <v>246</v>
       </c>
-      <c r="V5" s="201" t="s">
+      <c r="Y5" s="196" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z5" s="196" t="s">
         <v>248</v>
       </c>
-      <c r="W5" s="201" t="s">
-        <v>249</v>
-      </c>
-      <c r="X5" s="201" t="s">
-        <v>250</v>
-      </c>
-      <c r="Z5" s="149" t="s">
+      <c r="AB5" s="155" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC5" s="149" t="s">
         <v>230</v>
       </c>
-      <c r="AA5" s="149" t="s">
-        <v>242</v>
-      </c>
-      <c r="AB5" s="149" t="s">
-        <v>251</v>
-      </c>
-      <c r="AC5" s="149" t="s">
+      <c r="AD5" s="149" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="11:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="11:30" x14ac:dyDescent="0.25">
       <c r="K6" t="s">
         <v>201</v>
       </c>
       <c r="L6" s="190">
-        <v>487500</v>
-      </c>
-      <c r="M6" s="193">
-        <v>162500</v>
-      </c>
-      <c r="O6" s="150">
+        <v>74996</v>
+      </c>
+      <c r="M6" s="190">
+        <v>24988</v>
+      </c>
+      <c r="O6" s="203">
+        <v>6.5</v>
+      </c>
+      <c r="Q6" s="150">
         <f>SUMPRODUCT(L6:M6, $L$3:$M$3)</f>
-        <v>5200000</v>
-      </c>
-      <c r="P6" s="150" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q6" s="199">
-        <f>$T6 * SUM($L6,$M6)</f>
-        <v>5200000</v>
-      </c>
-      <c r="R6" s="185" t="b">
-        <f>O6 &gt;= Q6</f>
+        <v>799904</v>
+      </c>
+      <c r="R6" s="150" t="s">
+        <v>241</v>
+      </c>
+      <c r="S6" s="194">
+        <f>$V6 * SUM($L6,$M6)</f>
+        <v>799872</v>
+      </c>
+      <c r="T6" s="185" t="b">
+        <f>Q6 &gt;= S6</f>
         <v>1</v>
       </c>
-      <c r="T6" s="200">
+      <c r="V6" s="195">
         <v>8</v>
       </c>
-      <c r="V6" s="202">
+      <c r="X6" s="197">
         <f>L6 / SUM($L6:$M6)</f>
-        <v>0.75</v>
-      </c>
-      <c r="W6" s="202">
+        <v>0.75008001280204828</v>
+      </c>
+      <c r="Y6" s="197">
         <f>M6 / SUM($L6:$M6)</f>
-        <v>0.25</v>
-      </c>
-      <c r="X6" s="203">
-        <f>V6 * L$3 + W6 * M$3</f>
-        <v>8</v>
-      </c>
-      <c r="Z6" s="213">
+        <v>0.24991998719795167</v>
+      </c>
+      <c r="Z6" s="217">
+        <f>X6 * L$3 + Y6 * M$3</f>
+        <v>8.0003200512081918</v>
+      </c>
+      <c r="AB6" s="214" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC6" s="210">
         <v>0.35</v>
       </c>
-      <c r="AA6" s="210">
-        <v>6.5</v>
-      </c>
-      <c r="AB6" s="211">
-        <f t="shared" ref="AB6:AB8" si="1">Z6 / AA6</f>
-        <v>5.3846153846153842E-2</v>
-      </c>
-      <c r="AC6" s="212">
-        <f>AB6 * SUM(L6:M6)</f>
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="7" spans="11:29" x14ac:dyDescent="0.25">
+      <c r="AD6" s="204">
+        <f>AC6 * SUM(L6:M6)</f>
+        <v>34994.399999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="11:30" x14ac:dyDescent="0.25">
       <c r="K7" t="s">
         <v>191</v>
       </c>
-      <c r="L7" s="191">
-        <v>442500</v>
-      </c>
-      <c r="M7" s="194">
-        <v>1327500</v>
-      </c>
-      <c r="O7" s="150">
+      <c r="L7" s="190">
+        <v>31609</v>
+      </c>
+      <c r="M7" s="190">
+        <v>94827</v>
+      </c>
+      <c r="O7" s="191">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="150">
         <f>SUMPRODUCT(L7:M7, $L$3:$M$3)</f>
-        <v>10620000</v>
-      </c>
-      <c r="P7" s="150" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q7" s="199">
-        <f>$T7 * SUM($L7,$M7)</f>
-        <v>10620000</v>
-      </c>
-      <c r="R7" s="185" t="b">
-        <f>O7 &gt;= Q7</f>
+        <v>758616</v>
+      </c>
+      <c r="R7" s="150" t="s">
+        <v>241</v>
+      </c>
+      <c r="S7" s="194">
+        <f>$V7 * SUM($L7,$M7)</f>
+        <v>758616</v>
+      </c>
+      <c r="T7" s="185" t="b">
+        <f>Q7 &gt;= S7</f>
         <v>1</v>
       </c>
-      <c r="T7" s="200">
+      <c r="V7" s="195">
         <v>6</v>
       </c>
-      <c r="V7" s="202">
-        <f t="shared" ref="V7:V8" si="2">L7 / SUM($L7:$M7)</f>
+      <c r="X7" s="197">
+        <f t="shared" ref="X7:X8" si="1">L7 / SUM($L7:$M7)</f>
         <v>0.25</v>
       </c>
-      <c r="W7" s="202">
-        <f t="shared" ref="W7:W8" si="3">M7 / SUM($L7:$M7)</f>
+      <c r="Y7" s="197">
+        <f t="shared" ref="Y7:Y8" si="2">M7 / SUM($L7:$M7)</f>
         <v>0.75</v>
       </c>
-      <c r="X7" s="203">
-        <f>V7 * L$3 + W7 * M$3</f>
+      <c r="Z7" s="217">
+        <f>X7 * L$3 + Y7 * M$3</f>
         <v>6</v>
       </c>
-      <c r="Z7" s="214">
+      <c r="AB7" s="215" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC7" s="211">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="AA7" s="196">
-        <v>14</v>
-      </c>
-      <c r="AB7" s="204">
-        <f t="shared" si="1"/>
-        <v>-0.01</v>
-      </c>
-      <c r="AC7" s="205">
-        <f>AB7 * SUM(L7:M7)</f>
-        <v>-17700</v>
-      </c>
-    </row>
-    <row r="8" spans="11:29" x14ac:dyDescent="0.25">
+      <c r="AD7" s="198">
+        <f t="shared" ref="AD7:AD8" si="3">AC7 * SUM(L7:M7)</f>
+        <v>-17701.04</v>
+      </c>
+    </row>
+    <row r="8" spans="11:30" x14ac:dyDescent="0.25">
       <c r="K8" s="156" t="s">
         <v>192</v>
       </c>
-      <c r="L8" s="192">
+      <c r="L8" s="190">
         <v>0</v>
       </c>
-      <c r="M8" s="195">
-        <v>3780000</v>
-      </c>
-      <c r="O8" s="150">
+      <c r="M8" s="190">
+        <v>210000</v>
+      </c>
+      <c r="O8" s="192">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="150">
         <f>SUMPRODUCT(L8:M8, $L$3:$M$3)</f>
-        <v>18900000</v>
-      </c>
-      <c r="P8" s="150" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q8" s="199">
-        <f>$T8 * SUM($L8,$M8)</f>
+        <v>1050000</v>
+      </c>
+      <c r="R8" s="150" t="s">
+        <v>241</v>
+      </c>
+      <c r="S8" s="194">
+        <f>$V8 * SUM($L8,$M8)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="185" t="b">
-        <f>O8 &gt;= Q8</f>
+      <c r="T8" s="185" t="b">
+        <f>Q8 &gt;= S8</f>
         <v>1</v>
       </c>
-      <c r="T8" s="200">
+      <c r="V8" s="195">
         <v>0</v>
       </c>
-      <c r="V8" s="202">
+      <c r="X8" s="197">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y8" s="197">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="202">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="217">
+        <f>X8 * L$3 + Y8 * M$3</f>
+        <v>5</v>
+      </c>
+      <c r="AB8" s="216" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC8" s="212">
+        <v>0.43</v>
+      </c>
+      <c r="AD8" s="199">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="X8" s="203">
-        <f>V8 * L$3 + W8 * M$3</f>
-        <v>5</v>
-      </c>
-      <c r="Z8" s="215">
-        <v>0.43</v>
-      </c>
-      <c r="AA8" s="197">
-        <v>18</v>
-      </c>
-      <c r="AB8" s="211">
-        <f t="shared" si="1"/>
-        <v>2.388888888888889E-2</v>
-      </c>
-      <c r="AC8" s="206">
-        <f>AB8 * SUM(L8:M8)</f>
         <v>90300</v>
       </c>
     </row>
-    <row r="9" spans="11:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="11:30" x14ac:dyDescent="0.25">
       <c r="K9" s="148" t="s">
         <v>240</v>
       </c>
       <c r="L9" s="152">
-        <f>SUM(L6:L8)</f>
+        <f>SUMPRODUCT(L6:L8, $O$6:$O$8)</f>
         <v>930000</v>
       </c>
       <c r="M9" s="152">
-        <f>SUM(M6:M8)</f>
+        <f>SUMPRODUCT(M6:M8, $O$6:$O$8)</f>
         <v>5270000</v>
       </c>
-      <c r="O9" s="150"/>
-      <c r="P9" s="150"/>
-      <c r="Q9" s="199"/>
-      <c r="Z9" s="189"/>
-      <c r="AA9" s="189"/>
-      <c r="AB9" s="148" t="s">
-        <v>241</v>
-      </c>
-      <c r="AC9" s="207">
-        <f>SUM(AC6:AC8)</f>
-        <v>107600</v>
-      </c>
-    </row>
-    <row r="11" spans="11:29" ht="18" x14ac:dyDescent="0.35">
+      <c r="O9" s="189"/>
+      <c r="Q9" s="150"/>
+      <c r="R9" s="150"/>
+      <c r="S9" s="194"/>
+      <c r="AB9" s="213"/>
+      <c r="AC9" s="189"/>
+      <c r="AD9" s="200">
+        <f>SUM(AD6:AD8)</f>
+        <v>107593.35999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="11:30" ht="18" x14ac:dyDescent="0.35">
       <c r="K11" s="184" t="s">
-        <v>252</v>
-      </c>
-      <c r="L11" s="198">
+        <v>249</v>
+      </c>
+      <c r="L11" s="193">
         <f>SUM(L9:M9)</f>
         <v>6200000</v>
       </c>
-      <c r="O11" s="219" t="s">
-        <v>257</v>
-      </c>
-      <c r="P11" s="220" t="s">
-        <v>258</v>
-      </c>
+      <c r="Q11" s="208" t="s">
+        <v>254</v>
+      </c>
+      <c r="R11" s="209" t="s">
+        <v>255</v>
+      </c>
+      <c r="AB11" s="184"/>
+    </row>
+    <row r="14" spans="11:30" x14ac:dyDescent="0.25">
+      <c r="T14"/>
+    </row>
+    <row r="15" spans="11:30" x14ac:dyDescent="0.25">
+      <c r="T15"/>
+    </row>
+    <row r="16" spans="11:30" x14ac:dyDescent="0.25">
+      <c r="T16"/>
+    </row>
+    <row r="17" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T17"/>
+    </row>
+    <row r="18" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T18"/>
+    </row>
+    <row r="19" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T19"/>
+    </row>
+    <row r="20" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T20"/>
+    </row>
+    <row r="21" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T21"/>
+    </row>
+    <row r="22" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T22"/>
+    </row>
+    <row r="23" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T23"/>
+    </row>
+    <row r="24" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T24"/>
+    </row>
+    <row r="25" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T25"/>
+    </row>
+    <row r="26" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T26"/>
+    </row>
+    <row r="27" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T27"/>
+    </row>
+    <row r="28" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T28"/>
+    </row>
+    <row r="29" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T29"/>
+    </row>
+    <row r="30" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T30"/>
+    </row>
+    <row r="31" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add other model parameters
</commit_message>
<xml_diff>
--- a/03 - Homework/HW 02/Network Flow Graphs.xlsx
+++ b/03 - Homework/HW 02/Network Flow Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.carpenter\OneDrive - the Chickasaw Nation\Documents\GitHub\OU-DSA\Metaheuristics\03 - Homework\HW 02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87281062-8351-4C42-BC8F-6C3BF0EA7D6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8363AD-80C3-46E3-92F2-35BF3276F3B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EF627D34-B3C1-4C69-93C1-3362B4C646B4}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="261">
   <si>
     <t>Labor Sources</t>
   </si>
@@ -1521,6 +1521,21 @@
       <t>), for all p in PRODUCTS</t>
     </r>
   </si>
+  <si>
+    <t>gradeA</t>
+  </si>
+  <si>
+    <t>raisins</t>
+  </si>
+  <si>
+    <t>juice</t>
+  </si>
+  <si>
+    <t>jelly</t>
+  </si>
+  <si>
+    <t>gradeB</t>
+  </si>
 </sst>
 </file>
 
@@ -1535,7 +1550,7 @@
     <numFmt numFmtId="167" formatCode="&quot;(&quot;0&quot;,0,∞)&quot;"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="42" x14ac:knownFonts="1">
     <font>
@@ -3051,8 +3066,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="36" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="34" fillId="11" borderId="42" xfId="3" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="35" fillId="13" borderId="43" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3073,7 +3086,6 @@
     <xf numFmtId="0" fontId="36" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="39" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" wrapText="1"/>
@@ -3097,7 +3109,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="9" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="9" borderId="51" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -12461,7 +12476,7 @@
   <dimension ref="A2:AE31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -12527,15 +12542,15 @@
       <c r="R4" s="163"/>
       <c r="S4" s="163"/>
       <c r="T4" s="163"/>
-      <c r="X4" s="205" t="s">
+      <c r="X4" s="202" t="s">
         <v>252</v>
       </c>
-      <c r="Y4" s="205"/>
-      <c r="Z4" s="205"/>
-      <c r="AC4" s="206" t="s">
+      <c r="Y4" s="202"/>
+      <c r="Z4" s="202"/>
+      <c r="AC4" s="203" t="s">
         <v>253</v>
       </c>
-      <c r="AD4" s="207"/>
+      <c r="AD4" s="204"/>
     </row>
     <row r="5" spans="11:30" ht="30" x14ac:dyDescent="0.25">
       <c r="K5" s="149" t="s">
@@ -12550,26 +12565,26 @@
       <c r="O5" s="149" t="s">
         <v>193</v>
       </c>
-      <c r="Q5" s="201" t="s">
+      <c r="Q5" s="199" t="s">
         <v>242</v>
       </c>
-      <c r="R5" s="202"/>
-      <c r="S5" s="201" t="s">
+      <c r="R5" s="200"/>
+      <c r="S5" s="199" t="s">
         <v>243</v>
       </c>
-      <c r="T5" s="202" t="s">
+      <c r="T5" s="200" t="s">
         <v>250</v>
       </c>
       <c r="V5" s="155" t="s">
         <v>244</v>
       </c>
-      <c r="X5" s="196" t="s">
+      <c r="X5" s="194" t="s">
         <v>246</v>
       </c>
-      <c r="Y5" s="196" t="s">
+      <c r="Y5" s="194" t="s">
         <v>247</v>
       </c>
-      <c r="Z5" s="196" t="s">
+      <c r="Z5" s="194" t="s">
         <v>248</v>
       </c>
       <c r="AB5" s="155" t="s">
@@ -12587,53 +12602,55 @@
         <v>201</v>
       </c>
       <c r="L6" s="190">
-        <v>74996</v>
+        <f t="shared" ref="L6:L8" si="1">N17</f>
+        <v>40769</v>
       </c>
       <c r="M6" s="190">
-        <v>24988</v>
-      </c>
-      <c r="O6" s="203">
+        <f t="shared" ref="M6:M8" si="2">N20</f>
+        <v>13589</v>
+      </c>
+      <c r="O6" s="215">
         <v>6.5</v>
       </c>
       <c r="Q6" s="150">
         <f>SUMPRODUCT(L6:M6, $L$3:$M$3)</f>
-        <v>799904</v>
+        <v>434866</v>
       </c>
       <c r="R6" s="150" t="s">
         <v>241</v>
       </c>
-      <c r="S6" s="194">
+      <c r="S6" s="192">
         <f>$V6 * SUM($L6,$M6)</f>
-        <v>799872</v>
+        <v>434864</v>
       </c>
       <c r="T6" s="185" t="b">
         <f>Q6 &gt;= S6</f>
         <v>1</v>
       </c>
-      <c r="V6" s="195">
+      <c r="V6" s="193">
         <v>8</v>
       </c>
-      <c r="X6" s="197">
+      <c r="X6" s="195">
         <f>L6 / SUM($L6:$M6)</f>
-        <v>0.75008001280204828</v>
-      </c>
-      <c r="Y6" s="197">
+        <v>0.75000919827808232</v>
+      </c>
+      <c r="Y6" s="195">
         <f>M6 / SUM($L6:$M6)</f>
-        <v>0.24991998719795167</v>
-      </c>
-      <c r="Z6" s="217">
+        <v>0.24999080172191765</v>
+      </c>
+      <c r="Z6" s="214">
         <f>X6 * L$3 + Y6 * M$3</f>
-        <v>8.0003200512081918</v>
-      </c>
-      <c r="AB6" s="214" t="s">
+        <v>8.0000367931123293</v>
+      </c>
+      <c r="AB6" s="211" t="s">
         <v>201</v>
       </c>
-      <c r="AC6" s="210">
+      <c r="AC6" s="207">
         <v>0.35</v>
       </c>
-      <c r="AD6" s="204">
+      <c r="AD6" s="201">
         <f>AC6 * SUM(L6:M6)</f>
-        <v>34994.399999999994</v>
+        <v>19025.3</v>
       </c>
     </row>
     <row r="7" spans="11:30" x14ac:dyDescent="0.25">
@@ -12641,53 +12658,55 @@
         <v>191</v>
       </c>
       <c r="L7" s="190">
-        <v>31609</v>
+        <f t="shared" si="1"/>
+        <v>47500</v>
       </c>
       <c r="M7" s="190">
-        <v>94827</v>
-      </c>
-      <c r="O7" s="191">
+        <f t="shared" si="2"/>
+        <v>142499</v>
+      </c>
+      <c r="O7" s="216">
         <v>14</v>
       </c>
       <c r="Q7" s="150">
         <f>SUMPRODUCT(L7:M7, $L$3:$M$3)</f>
-        <v>758616</v>
+        <v>1139995</v>
       </c>
       <c r="R7" s="150" t="s">
         <v>241</v>
       </c>
-      <c r="S7" s="194">
+      <c r="S7" s="192">
         <f>$V7 * SUM($L7,$M7)</f>
-        <v>758616</v>
+        <v>1139994</v>
       </c>
       <c r="T7" s="185" t="b">
         <f>Q7 &gt;= S7</f>
         <v>1</v>
       </c>
-      <c r="V7" s="195">
+      <c r="V7" s="193">
         <v>6</v>
       </c>
-      <c r="X7" s="197">
-        <f t="shared" ref="X7:X8" si="1">L7 / SUM($L7:$M7)</f>
-        <v>0.25</v>
-      </c>
-      <c r="Y7" s="197">
-        <f t="shared" ref="Y7:Y8" si="2">M7 / SUM($L7:$M7)</f>
-        <v>0.75</v>
-      </c>
-      <c r="Z7" s="217">
+      <c r="X7" s="195">
+        <f t="shared" ref="X7:X8" si="3">L7 / SUM($L7:$M7)</f>
+        <v>0.25000131579639895</v>
+      </c>
+      <c r="Y7" s="195">
+        <f t="shared" ref="Y7:Y8" si="4">M7 / SUM($L7:$M7)</f>
+        <v>0.74999868420360105</v>
+      </c>
+      <c r="Z7" s="214">
         <f>X7 * L$3 + Y7 * M$3</f>
-        <v>6</v>
-      </c>
-      <c r="AB7" s="215" t="s">
+        <v>6.0000052631855958</v>
+      </c>
+      <c r="AB7" s="212" t="s">
         <v>191</v>
       </c>
-      <c r="AC7" s="211">
+      <c r="AC7" s="208">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="AD7" s="198">
-        <f t="shared" ref="AD7:AD8" si="3">AC7 * SUM(L7:M7)</f>
-        <v>-17701.04</v>
+      <c r="AD7" s="196">
+        <f t="shared" ref="AD7:AD8" si="5">AC7 * SUM(L7:M7)</f>
+        <v>-26599.860000000004</v>
       </c>
     </row>
     <row r="8" spans="11:30" x14ac:dyDescent="0.25">
@@ -12695,22 +12714,24 @@
         <v>192</v>
       </c>
       <c r="L8" s="190">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M8" s="190">
-        <v>210000</v>
-      </c>
-      <c r="O8" s="192">
+        <f t="shared" si="2"/>
+        <v>177038</v>
+      </c>
+      <c r="O8" s="217">
         <v>18</v>
       </c>
       <c r="Q8" s="150">
         <f>SUMPRODUCT(L8:M8, $L$3:$M$3)</f>
-        <v>1050000</v>
+        <v>885190</v>
       </c>
       <c r="R8" s="150" t="s">
         <v>241</v>
       </c>
-      <c r="S8" s="194">
+      <c r="S8" s="192">
         <f>$V8 * SUM($L8,$M8)</f>
         <v>0</v>
       </c>
@@ -12718,30 +12739,30 @@
         <f>Q8 &gt;= S8</f>
         <v>1</v>
       </c>
-      <c r="V8" s="195">
+      <c r="V8" s="193">
         <v>0</v>
       </c>
-      <c r="X8" s="197">
-        <f t="shared" si="1"/>
+      <c r="X8" s="195">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Y8" s="197">
-        <f t="shared" si="2"/>
+      <c r="Y8" s="195">
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Z8" s="217">
+      <c r="Z8" s="214">
         <f>X8 * L$3 + Y8 * M$3</f>
         <v>5</v>
       </c>
-      <c r="AB8" s="216" t="s">
+      <c r="AB8" s="213" t="s">
         <v>192</v>
       </c>
-      <c r="AC8" s="212">
+      <c r="AC8" s="209">
         <v>0.43</v>
       </c>
-      <c r="AD8" s="199">
-        <f t="shared" si="3"/>
-        <v>90300</v>
+      <c r="AD8" s="197">
+        <f t="shared" si="5"/>
+        <v>76126.34</v>
       </c>
     </row>
     <row r="9" spans="11:30" x14ac:dyDescent="0.25">
@@ -12750,35 +12771,35 @@
       </c>
       <c r="L9" s="152">
         <f>SUMPRODUCT(L6:L8, $O$6:$O$8)</f>
-        <v>930000</v>
+        <v>929998.5</v>
       </c>
       <c r="M9" s="152">
         <f>SUMPRODUCT(M6:M8, $O$6:$O$8)</f>
-        <v>5270000</v>
+        <v>5269998.5</v>
       </c>
       <c r="O9" s="189"/>
       <c r="Q9" s="150"/>
       <c r="R9" s="150"/>
-      <c r="S9" s="194"/>
-      <c r="AB9" s="213"/>
+      <c r="S9" s="192"/>
+      <c r="AB9" s="210"/>
       <c r="AC9" s="189"/>
-      <c r="AD9" s="200">
+      <c r="AD9" s="198">
         <f>SUM(AD6:AD8)</f>
-        <v>107593.35999999999</v>
+        <v>68551.78</v>
       </c>
     </row>
     <row r="11" spans="11:30" ht="18" x14ac:dyDescent="0.35">
       <c r="K11" s="184" t="s">
         <v>249</v>
       </c>
-      <c r="L11" s="193">
+      <c r="L11" s="191">
         <f>SUM(L9:M9)</f>
-        <v>6200000</v>
-      </c>
-      <c r="Q11" s="208" t="s">
+        <v>6199997</v>
+      </c>
+      <c r="Q11" s="205" t="s">
         <v>254</v>
       </c>
-      <c r="R11" s="209" t="s">
+      <c r="R11" s="206" t="s">
         <v>255</v>
       </c>
       <c r="AB11" s="184"/>
@@ -12792,49 +12813,103 @@
     <row r="16" spans="11:30" x14ac:dyDescent="0.25">
       <c r="T16"/>
     </row>
-    <row r="17" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:20" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>256</v>
+      </c>
+      <c r="M17" t="s">
+        <v>257</v>
+      </c>
+      <c r="N17">
+        <v>40769</v>
+      </c>
       <c r="T17"/>
     </row>
-    <row r="18" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="12:20" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>256</v>
+      </c>
+      <c r="M18" t="s">
+        <v>258</v>
+      </c>
+      <c r="N18">
+        <v>47500</v>
+      </c>
       <c r="T18"/>
     </row>
-    <row r="19" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="12:20" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>256</v>
+      </c>
+      <c r="M19" t="s">
+        <v>259</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
       <c r="T19"/>
     </row>
-    <row r="20" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="12:20" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>260</v>
+      </c>
+      <c r="M20" t="s">
+        <v>257</v>
+      </c>
+      <c r="N20">
+        <v>13589</v>
+      </c>
       <c r="T20"/>
     </row>
-    <row r="21" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="12:20" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>260</v>
+      </c>
+      <c r="M21" t="s">
+        <v>258</v>
+      </c>
+      <c r="N21">
+        <v>142499</v>
+      </c>
       <c r="T21"/>
     </row>
-    <row r="22" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="12:20" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>260</v>
+      </c>
+      <c r="M22" t="s">
+        <v>259</v>
+      </c>
+      <c r="N22">
+        <v>177038</v>
+      </c>
       <c r="T22"/>
     </row>
-    <row r="23" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="12:20" x14ac:dyDescent="0.25">
       <c r="T23"/>
     </row>
-    <row r="24" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="12:20" x14ac:dyDescent="0.25">
       <c r="T24"/>
     </row>
-    <row r="25" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="12:20" x14ac:dyDescent="0.25">
       <c r="T25"/>
     </row>
-    <row r="26" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="12:20" x14ac:dyDescent="0.25">
       <c r="T26"/>
     </row>
-    <row r="27" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="12:20" x14ac:dyDescent="0.25">
       <c r="T27"/>
     </row>
-    <row r="28" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="12:20" x14ac:dyDescent="0.25">
       <c r="T28"/>
     </row>
-    <row r="29" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="12:20" x14ac:dyDescent="0.25">
       <c r="T29"/>
     </row>
-    <row r="30" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="12:20" x14ac:dyDescent="0.25">
       <c r="T30"/>
     </row>
-    <row r="31" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="12:20" x14ac:dyDescent="0.25">
       <c r="T31"/>
     </row>
   </sheetData>

</xml_diff>